<commit_message>
Status Words & CAN
created a status word (32 bits) for inputs and controller and packed them for CAN usage
Implemented the BClutchEngaged flag
Defined and implemented the CAN messages
</commit_message>
<xml_diff>
--- a/Docs/P19_Maps_v01.xlsx
+++ b/Docs/P19_Maps_v01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03.CODE\P19-Shifter\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAB25A3-F337-4FA7-8F9B-E8BFC3879186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71BFBC9-4E86-485D-BC06-A011BD6F5C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{B721293F-9984-497B-84C2-5BF522F68054}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{B721293F-9984-497B-84C2-5BF522F68054}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -98,13 +98,109 @@
   </si>
   <si>
     <t>0x311</t>
+  </si>
+  <si>
+    <t>Bit0: BUpShiftButtonInError    Bit1: BDnShiftButtonInError   Bit2: 0                                                           Bit3: 0                                                           Bit4: 0                                                           Bit5: 0                                                           Bit6: BrClutchPaddleInError                                          Bit7: 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit0: BUpShiftButtonPressed   Bit1: BDnShiftButtonPressed    Bit2: BButtonAPressed                                                            Bit3: BButtonBPressed                                                         Bit4: BButtonCPressed                                                              Bit5: BButtonDPressed                                                                  Bit6: BButtonEPressed                                                  Bit7: BButtonFPressed        </t>
+  </si>
+  <si>
+    <t>rClutchPaddle  (in8_t) (-128-128)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>rmp</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>0x321</t>
+  </si>
+  <si>
+    <t>multifunction maps for ECU</t>
+  </si>
+  <si>
+    <t>CAN Errors</t>
+  </si>
+  <si>
+    <t>0x322</t>
+  </si>
+  <si>
+    <t>INPUT FLAGS           [bit7-bit0]</t>
+  </si>
+  <si>
+    <t>INPUT FLAGS           [bit15-bit8]</t>
+  </si>
+  <si>
+    <t>INPUT FLAGS           [bit23-bit16]</t>
+  </si>
+  <si>
+    <t>INPUT FLAGS           [bit31-bit24]</t>
+  </si>
+  <si>
+    <t>CONTROLLER FLAGS           [bit7-bit0]</t>
+  </si>
+  <si>
+    <t>CONTROLLER FLAGS           [bit15-bit8]</t>
+  </si>
+  <si>
+    <t>CONTROLLER FLAGS           [bit23-bit16]</t>
+  </si>
+  <si>
+    <t>CONTROLLER FLAGS           [bit31-bit24]</t>
+  </si>
+  <si>
+    <t>see details for the flags on the screenshots</t>
+  </si>
+  <si>
+    <t>NGear                          (uint8_t)</t>
+  </si>
+  <si>
+    <t>rClutchPaddle Echo (int8_t)</t>
+  </si>
+  <si>
+    <t>Display &amp; LEDS Flag</t>
+  </si>
+  <si>
+    <t>nEngine Echo          (MSB)</t>
+  </si>
+  <si>
+    <t>nEngine Echo          (LSB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Vsupply: (divide by 1000 and cast to float)               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vsupply                                    (MSB) </t>
+  </si>
+  <si>
+    <t>Vsupply                                                                                  (LSB)</t>
+  </si>
+  <si>
+    <t>CAN Rx Errors</t>
+  </si>
+  <si>
+    <t>Reserved for ECU Control</t>
+  </si>
+  <si>
+    <t>xClutchTarget                      (MSB)</t>
+  </si>
+  <si>
+    <t>xClutchTarget                      (LSB)</t>
+  </si>
+  <si>
+    <t>Display Page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,16 +214,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -252,19 +382,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -409,11 +526,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -436,47 +577,107 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,23 +700,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>34624</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>457138</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>161578</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>365215</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>58025</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B2040BE-F9E4-D3A8-5719-BE0C44CE4236}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DAFE1B6-E545-314E-6601-422B06BF9036}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -531,8 +732,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13596257" y="589795"/>
-          <a:ext cx="5878224" cy="4584654"/>
+          <a:off x="14142720" y="746760"/>
+          <a:ext cx="9745435" cy="6268325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -543,23 +744,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>424543</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>157280</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>373379</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>33944</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>144409</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>34358</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0196174-F587-9269-7737-4DFE899BDF5F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE3A0D01-2ECF-964B-0A95-8F4AB4737D23}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -575,8 +776,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13563600" y="5355209"/>
-          <a:ext cx="6793973" cy="912414"/>
+          <a:off x="15262859" y="7117080"/>
+          <a:ext cx="10024179" cy="5082540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1005840</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2656269</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>50017</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AA8232C-F4DB-6072-97C7-8E5E24F91B5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9738360" y="5715000"/>
+          <a:ext cx="5010849" cy="3486637"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -909,7 +1154,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -917,354 +1162,463 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFD32C5-AC0D-4462-82E8-BCB5DEF54875}">
-  <dimension ref="D4:P23"/>
+  <dimension ref="B4:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="15" width="9.23046875" style="1"/>
-    <col min="16" max="16" width="47.23046875" style="1" customWidth="1"/>
+    <col min="2" max="4" width="9.21875" style="1"/>
+    <col min="5" max="5" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.21875" style="1" customWidth="1"/>
+    <col min="10" max="13" width="16.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="40.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="5" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D5" s="11" t="s">
+    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="C5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="D5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="E5" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="F5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="G5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="H5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="I5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="J5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="K5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="L5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="18" t="s">
+      <c r="M5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="13" t="s">
+      <c r="N5" s="25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D6" s="8" t="s">
+    <row r="6" spans="2:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="B6" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="C6" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="9">
+      <c r="D6" s="36">
         <v>8</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="10"/>
-    </row>
-    <row r="7" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D7" s="3"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="2">
+      <c r="E6" s="37">
+        <v>100</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="30"/>
+      <c r="C7" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="12">
         <v>8</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D8" s="3"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D9" s="3" t="s">
+      <c r="E7" s="27">
+        <v>100</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="31"/>
+      <c r="C8" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="12">
+        <v>8</v>
+      </c>
+      <c r="E8" s="27">
+        <v>100</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="N8" s="34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" s="13" customFormat="1" ht="76.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="C9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="2">
+      <c r="D9" s="12">
         <v>8</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D10" s="3"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="4"/>
-    </row>
-    <row r="11" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D11" s="3"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="4"/>
-    </row>
-    <row r="12" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D12" s="3" t="s">
+      <c r="E9" s="27">
+        <v>100</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B11" s="3"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="C12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="2">
+      <c r="D12" s="2">
         <v>8</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="4"/>
-    </row>
-    <row r="13" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D13" s="3"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="4"/>
-    </row>
-    <row r="14" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D14" s="3"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="4"/>
-    </row>
-    <row r="15" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D15" s="3"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="4"/>
-    </row>
-    <row r="16" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D16" s="3"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="4"/>
-    </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D17" s="3"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="4"/>
-    </row>
-    <row r="18" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D18" s="3"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="4"/>
-    </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D19" s="3"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="4"/>
-    </row>
-    <row r="20" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D20" s="3"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="4"/>
-    </row>
-    <row r="21" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D21" s="3"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="4"/>
-    </row>
-    <row r="22" spans="4:16" x14ac:dyDescent="0.4">
-      <c r="D22" s="3"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="4"/>
-    </row>
-    <row r="23" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D23" s="5"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="21"/>
-      <c r="P23" s="7"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="3"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="3"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="3"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="3"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B17" s="3"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="3"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="3"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="3"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" s="3"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B22" s="3"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="5"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="7"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:B8"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1276,7 +1630,7 @@
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1288,7 +1642,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1300,7 +1654,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1312,7 +1666,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Display pages & More multifunction & Toggles
Defined the change page on multifunction and errors strategy
added the override option for each multifunction, in order to block it for potential toggle usage and or other blocking strategies
moved the toggle function for the inputs to the controller
</commit_message>
<xml_diff>
--- a/Docs/P19_Maps_v01.xlsx
+++ b/Docs/P19_Maps_v01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03.CODE\P19-Shifter\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6671832-B85D-41EC-B314-90D90CAC4306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4C5FB7-C682-405B-8ED5-E35A5957C23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{B721293F-9984-497B-84C2-5BF522F68054}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{B721293F-9984-497B-84C2-5BF522F68054}"/>
   </bookViews>
   <sheets>
     <sheet name="CAN" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -258,7 +258,22 @@
     <t>Clutch Target</t>
   </si>
   <si>
-    <t>knee Point</t>
+    <t>knee point 40%</t>
+  </si>
+  <si>
+    <t>Gain (first)</t>
+  </si>
+  <si>
+    <t>knee point 30%</t>
+  </si>
+  <si>
+    <t>knee point 20%</t>
+  </si>
+  <si>
+    <t>Unprogressive 2</t>
+  </si>
+  <si>
+    <t>knee point 50%</t>
   </si>
 </sst>
 </file>
@@ -323,10 +338,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -789,6 +802,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -798,14 +817,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2674,6 +2685,490 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1955292544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ClutchPaddle</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Map 12</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" baseline="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ClutchPaddle!$C$231:$C$241</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ClutchPaddle!$D$231:$D$241</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1060</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CEEB-41F6-BEF8-5EA0EB7AEBFC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1955292544"/>
+        <c:axId val="1955299072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1955292544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="101"/>
+          <c:min val="-1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>rClutchPaddle</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1955299072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1955299072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="800"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>xClutchTargetManual</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6763,6 +7258,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -9147,7 +9682,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9663,7 +10198,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10179,7 +10714,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10695,7 +11230,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -11211,7 +11746,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -11727,7 +12262,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12243,7 +12778,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12759,7 +13294,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -13275,96 +13810,524 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>365215</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>58025</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DAFE1B6-E545-314E-6601-422B06BF9036}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14142720" y="746760"/>
-          <a:ext cx="9745435" cy="6268325"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>373379</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>34358</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE3A0D01-2ECF-964B-0A95-8F4AB4737D23}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15262859" y="7117080"/>
-          <a:ext cx="10024179" cy="5082540"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -13392,7 +14355,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -13436,7 +14399,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -13445,6 +14408,94 @@
         <a:xfrm>
           <a:off x="6774180" y="5585460"/>
           <a:ext cx="8125959" cy="4486901"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>421748</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>124577</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>40736</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C2F2892-D839-E085-59B4-FAC7580789FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15792377" y="636814"/>
+          <a:ext cx="10806257" cy="6517736"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>375556</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>143258</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>328556</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>181983</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DAC3B31-43EF-8CA6-8425-1CC4739A4A61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15746185" y="7257072"/>
+          <a:ext cx="13015857" cy="3924925"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13914,6 +14965,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>375012</xdr:colOff>
+      <xdr:row>226</xdr:row>
+      <xdr:rowOff>168319</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>531222</xdr:colOff>
+      <xdr:row>242</xdr:row>
+      <xdr:rowOff>58781</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C954CCC3-C8CE-2CE3-576D-D5214EDCFCE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -14236,23 +15325,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFD32C5-AC0D-4462-82E8-BCB5DEF54875}">
   <dimension ref="B4:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="4" width="9.21875" style="1"/>
-    <col min="5" max="5" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="16.21875" style="1" customWidth="1"/>
-    <col min="10" max="13" width="16.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="40.77734375" style="1" customWidth="1"/>
+    <col min="2" max="4" width="9.23046875" style="1"/>
+    <col min="5" max="5" width="9.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.23046875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.23046875" style="1" customWidth="1"/>
+    <col min="10" max="13" width="16.3046875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="40.765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B5" s="21" t="s">
         <v>10</v>
       </c>
@@ -14293,8 +15382,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="B6" s="47" t="s">
+    <row r="6" spans="2:14" ht="24" x14ac:dyDescent="0.4">
+      <c r="B6" s="51" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="32" t="s">
@@ -14334,8 +15423,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="48"/>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B7" s="52"/>
       <c r="C7" s="32" t="s">
         <v>24</v>
       </c>
@@ -14373,8 +15462,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="48"/>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B8" s="52"/>
       <c r="C8" s="32" t="s">
         <v>26</v>
       </c>
@@ -14410,8 +15499,8 @@
       </c>
       <c r="N8" s="31"/>
     </row>
-    <row r="9" spans="2:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="49"/>
+    <row r="9" spans="2:14" ht="25.75" x14ac:dyDescent="0.4">
+      <c r="B9" s="53"/>
       <c r="C9" s="32" t="s">
         <v>51</v>
       </c>
@@ -14449,7 +15538,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="2:14" s="13" customFormat="1" ht="76.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.4">
       <c r="B10" s="10" t="s">
         <v>13</v>
       </c>
@@ -14490,7 +15579,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B11" s="3"/>
       <c r="C11" s="8"/>
       <c r="D11" s="2"/>
@@ -14505,7 +15594,7 @@
       <c r="M11" s="15"/>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B12" s="3"/>
       <c r="C12" s="8"/>
       <c r="D12" s="2"/>
@@ -14520,7 +15609,7 @@
       <c r="M12" s="15"/>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
@@ -14547,7 +15636,7 @@
       <c r="M13" s="15"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B14" s="3"/>
       <c r="C14" s="8"/>
       <c r="D14" s="2"/>
@@ -14562,7 +15651,7 @@
       <c r="M14" s="15"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B15" s="3"/>
       <c r="C15" s="8"/>
       <c r="D15" s="2"/>
@@ -14577,7 +15666,7 @@
       <c r="M15" s="15"/>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B16" s="3"/>
       <c r="C16" s="8"/>
       <c r="D16" s="2"/>
@@ -14592,7 +15681,7 @@
       <c r="M16" s="15"/>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B17" s="3"/>
       <c r="C17" s="8"/>
       <c r="D17" s="2"/>
@@ -14607,7 +15696,7 @@
       <c r="M17" s="15"/>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B18" s="3"/>
       <c r="C18" s="8"/>
       <c r="D18" s="2"/>
@@ -14622,7 +15711,7 @@
       <c r="M18" s="15"/>
       <c r="N18" s="4"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B19" s="3"/>
       <c r="C19" s="8"/>
       <c r="D19" s="2"/>
@@ -14637,7 +15726,7 @@
       <c r="M19" s="15"/>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B20" s="3"/>
       <c r="C20" s="8"/>
       <c r="D20" s="2"/>
@@ -14652,7 +15741,7 @@
       <c r="M20" s="15"/>
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B21" s="3"/>
       <c r="C21" s="8"/>
       <c r="D21" s="2"/>
@@ -14667,7 +15756,7 @@
       <c r="M21" s="15"/>
       <c r="N21" s="4"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B22" s="3"/>
       <c r="C22" s="8"/>
       <c r="D22" s="2"/>
@@ -14682,7 +15771,7 @@
       <c r="M22" s="15"/>
       <c r="N22" s="4"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B23" s="3"/>
       <c r="C23" s="8"/>
       <c r="D23" s="2"/>
@@ -14697,7 +15786,7 @@
       <c r="M23" s="15"/>
       <c r="N23" s="4"/>
     </row>
-    <row r="24" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="5"/>
       <c r="C24" s="9"/>
       <c r="D24" s="6"/>
@@ -14725,22 +15814,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327977B7-E239-49BB-B0DD-EEBF381339C3}">
-  <dimension ref="A1:F224"/>
+  <dimension ref="A1:F244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+    <sheetView topLeftCell="A212" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q224" sqref="Q224"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.4609375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3046875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B1" s="2" t="s">
         <v>69</v>
       </c>
@@ -14748,7 +15837,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="41" t="s">
         <v>71</v>
       </c>
@@ -14759,7 +15848,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -14767,7 +15856,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C6" s="2" t="s">
         <v>54</v>
       </c>
@@ -14775,7 +15864,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C7" s="2">
         <v>0</v>
       </c>
@@ -14788,7 +15877,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C8" s="2">
         <f>C7+10</f>
         <v>10</v>
@@ -14798,7 +15887,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C9" s="2">
         <f t="shared" ref="C9:C17" si="0">C8+10</f>
         <v>20</v>
@@ -14808,7 +15897,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -14818,7 +15907,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -14828,7 +15917,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -14838,7 +15927,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -14848,7 +15937,7 @@
         <v>1620</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>70</v>
@@ -14858,7 +15947,7 @@
         <v>1740</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>80</v>
@@ -14868,7 +15957,7 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>90</v>
@@ -14878,7 +15967,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -14888,38 +15977,41 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C20" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="52" t="str">
+      <c r="D20" s="48" t="str">
         <f>"{"&amp;ROUND(D7,0)&amp;", "&amp;ROUND(D8,0)&amp;", "&amp;ROUND(D9,0)&amp;", "&amp;ROUND(D10,0)&amp;", "&amp;ROUND(D11,0)&amp;", "&amp;ROUND(D12,0)&amp;", "&amp;ROUND(D13,0)&amp;", "&amp;ROUND(D14,0)&amp;", "&amp;ROUND(D15,0)&amp;", "&amp;ROUND(D16,0)&amp;", "&amp;ROUND(D17,0)&amp;"}"</f>
         <v>{900, 1020, 1140, 1260, 1380, 1500, 1620, 1740, 1860, 1980, 2100}</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="C24" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="E24" s="41" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C25" s="2" t="s">
         <v>54</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E25" s="53">
+      <c r="E25" s="49">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C26" s="2">
         <v>0</v>
       </c>
@@ -14936,7 +16028,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C27" s="2">
         <f>C26+10</f>
         <v>10</v>
@@ -14954,7 +16046,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C28" s="2">
         <f t="shared" ref="C28:C36" si="2">C27+10</f>
         <v>20</v>
@@ -14963,7 +16055,7 @@
         <f t="shared" ref="D28:D30" si="3">C28*$E$25+$D$26</f>
         <v>1300</v>
       </c>
-      <c r="E28" s="50">
+      <c r="E28" s="47">
         <f>SLOPE(F26:F27,E26:E27)</f>
         <v>6.666666666666667</v>
       </c>
@@ -14972,7 +16064,7 @@
         <v>1433.3333333333333</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C29" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -14982,8 +16074,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C30" s="51">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C30" s="2">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
@@ -14992,7 +16084,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C31" s="2">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -15002,7 +16094,7 @@
         <v>1766.6666666666665</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C32" s="2">
         <f t="shared" si="2"/>
         <v>60</v>
@@ -15012,7 +16104,7 @@
         <v>1833.3333333333333</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C33" s="2">
         <f t="shared" si="2"/>
         <v>70</v>
@@ -15022,7 +16114,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C34" s="2">
         <f t="shared" si="2"/>
         <v>80</v>
@@ -15032,7 +16124,7 @@
         <v>1966.6666666666665</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C35" s="2">
         <f t="shared" si="2"/>
         <v>90</v>
@@ -15042,7 +16134,7 @@
         <v>2033.3333333333333</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C36" s="2">
         <f t="shared" si="2"/>
         <v>100</v>
@@ -15052,38 +16144,41 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C39" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D39" s="52" t="str">
+      <c r="D39" s="48" t="str">
         <f>"{"&amp;ROUND(D26,0)&amp;", "&amp;ROUND(D27,0)&amp;", "&amp;ROUND(D28,0)&amp;", "&amp;ROUND(D29,0)&amp;", "&amp;ROUND(D30,0)&amp;", "&amp;ROUND(D31,0)&amp;", "&amp;ROUND(D32,0)&amp;", "&amp;ROUND(D33,0)&amp;", "&amp;ROUND(D34,0)&amp;", "&amp;ROUND(D35,0)&amp;", "&amp;ROUND(D36,0)&amp;"}"</f>
         <v>{900, 1100, 1300, 1500, 1700, 1767, 1833, 1900, 1967, 2033, 2100}</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>3</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="C42" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E42" s="41" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C43" s="2" t="s">
         <v>54</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E43" s="53">
+      <c r="E43" s="49">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C44" s="2">
         <v>0</v>
       </c>
@@ -15100,7 +16195,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C45" s="2">
         <f>C44+10</f>
         <v>10</v>
@@ -15118,7 +16213,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C46" s="2">
         <f t="shared" ref="C46:C54" si="5">C45+10</f>
         <v>20</v>
@@ -15127,7 +16222,7 @@
         <f t="shared" ref="D46:D47" si="6">C46*$E$43+$D$44</f>
         <v>1500</v>
       </c>
-      <c r="E46" s="50">
+      <c r="E46" s="47">
         <f>SLOPE(F44:F45,E44:E45)</f>
         <v>4.2857142857142856</v>
       </c>
@@ -15136,8 +16231,8 @@
         <v>1671.4285714285716</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C47" s="51">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C47" s="2">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
@@ -15146,7 +16241,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C48" s="2">
         <f t="shared" si="5"/>
         <v>40</v>
@@ -15156,7 +16251,7 @@
         <v>1842.8571428571429</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C49" s="2">
         <f t="shared" si="5"/>
         <v>50</v>
@@ -15166,7 +16261,7 @@
         <v>1885.7142857142858</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C50" s="2">
         <f t="shared" si="5"/>
         <v>60</v>
@@ -15176,7 +16271,7 @@
         <v>1928.5714285714287</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C51" s="2">
         <f t="shared" si="5"/>
         <v>70</v>
@@ -15186,7 +16281,7 @@
         <v>1971.4285714285716</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C52" s="2">
         <f t="shared" si="5"/>
         <v>80</v>
@@ -15196,7 +16291,7 @@
         <v>2014.2857142857144</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C53" s="2">
         <f t="shared" si="5"/>
         <v>90</v>
@@ -15206,7 +16301,7 @@
         <v>2057.1428571428573</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C54" s="2">
         <f t="shared" si="5"/>
         <v>100</v>
@@ -15216,38 +16311,41 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C57" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D57" s="52" t="str">
+      <c r="D57" s="48" t="str">
         <f>"{"&amp;ROUND(D44,0)&amp;", "&amp;ROUND(D45,0)&amp;", "&amp;ROUND(D46,0)&amp;", "&amp;ROUND(D47,0)&amp;", "&amp;ROUND(D48,0)&amp;", "&amp;ROUND(D49,0)&amp;", "&amp;ROUND(D50,0)&amp;", "&amp;ROUND(D51,0)&amp;", "&amp;ROUND(D52,0)&amp;", "&amp;ROUND(D53,0)&amp;", "&amp;ROUND(D54,0)&amp;"}"</f>
         <v>{900, 1200, 1500, 1800, 1843, 1886, 1929, 1971, 2014, 2057, 2100}</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>4</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="C62" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="E62" s="41" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C63" s="2" t="s">
         <v>54</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="53">
+      <c r="E63" s="49">
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C64" s="2">
         <v>0</v>
       </c>
@@ -15264,7 +16362,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C65" s="2">
         <f>C64+10</f>
         <v>10</v>
@@ -15282,8 +16380,8 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C66" s="51">
+    <row r="66" spans="3:6" x14ac:dyDescent="0.4">
+      <c r="C66" s="2">
         <f t="shared" ref="C66:C74" si="8">C65+10</f>
         <v>20</v>
       </c>
@@ -15291,7 +16389,7 @@
         <f>C66*$E$63 +$D$64</f>
         <v>1800</v>
       </c>
-      <c r="E66" s="50">
+      <c r="E66" s="47">
         <f>SLOPE(F64:F65,E64:E65)</f>
         <v>3.75</v>
       </c>
@@ -15300,7 +16398,7 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C67" s="2">
         <f t="shared" si="8"/>
         <v>30</v>
@@ -15310,7 +16408,7 @@
         <v>1837.5</v>
       </c>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C68" s="2">
         <f t="shared" si="8"/>
         <v>40</v>
@@ -15320,7 +16418,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C69" s="2">
         <f t="shared" si="8"/>
         <v>50</v>
@@ -15330,7 +16428,7 @@
         <v>1912.5</v>
       </c>
     </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C70" s="2">
         <f t="shared" si="8"/>
         <v>60</v>
@@ -15340,7 +16438,7 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C71" s="2">
         <f t="shared" si="8"/>
         <v>70</v>
@@ -15350,7 +16448,7 @@
         <v>1987.5</v>
       </c>
     </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C72" s="2">
         <f t="shared" si="8"/>
         <v>80</v>
@@ -15360,7 +16458,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C73" s="2">
         <f t="shared" si="8"/>
         <v>90</v>
@@ -15370,7 +16468,7 @@
         <v>2062.5</v>
       </c>
     </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C74" s="2">
         <f t="shared" si="8"/>
         <v>100</v>
@@ -15380,16 +16478,16 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:6" x14ac:dyDescent="0.4">
       <c r="C77" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D77" s="52" t="str">
+      <c r="D77" s="48" t="str">
         <f>"{"&amp;ROUND(D64,0)&amp;", "&amp;ROUND(D65,0)&amp;", "&amp;ROUND(D66,0)&amp;", "&amp;ROUND(D67,0)&amp;", "&amp;ROUND(D68,0)&amp;", "&amp;ROUND(D69,0)&amp;", "&amp;ROUND(D70,0)&amp;", "&amp;ROUND(D71,0)&amp;", "&amp;ROUND(D72,0)&amp;", "&amp;ROUND(D73,0)&amp;", "&amp;ROUND(D74,0)&amp;"}"</f>
         <v>{900, 1350, 1800, 1838, 1875, 1913, 1950, 1988, 2025, 2063, 2100}</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>5</v>
       </c>
@@ -15397,7 +16495,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C83" s="2" t="s">
         <v>54</v>
       </c>
@@ -15405,7 +16503,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C84" s="2">
         <v>0</v>
       </c>
@@ -15413,46 +16511,52 @@
         <f>$B$2</f>
         <v>900</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E84" s="50">
+        <f>(D91-D86)/5</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C85" s="2">
         <f>C84+10</f>
         <v>10</v>
       </c>
       <c r="D85" s="44">
+        <f>D84</f>
         <v>900</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C86" s="2">
         <f t="shared" ref="C86:C94" si="10">C85+10</f>
         <v>20</v>
       </c>
       <c r="D86" s="44">
+        <f>D85</f>
         <v>900</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C87" s="2">
         <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="D87" s="44">
-        <f>D86+240</f>
+        <f>D86+$E$84</f>
         <v>1140</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C88" s="2">
         <f t="shared" si="10"/>
         <v>40</v>
       </c>
       <c r="D88" s="44">
-        <f t="shared" ref="D88:D91" si="11">D87+240</f>
+        <f t="shared" ref="D88:D90" si="11">D87+$E$84</f>
         <v>1380</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C89" s="2">
         <f t="shared" si="10"/>
         <v>50</v>
@@ -15462,7 +16566,7 @@
         <v>1620</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C90" s="2">
         <f t="shared" si="10"/>
         <v>60</v>
@@ -15472,35 +16576,37 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C91" s="2">
         <f t="shared" si="10"/>
         <v>70</v>
       </c>
       <c r="D91" s="44">
-        <f t="shared" si="11"/>
+        <f>D94</f>
         <v>2100</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C92" s="2">
         <f t="shared" si="10"/>
         <v>80</v>
       </c>
       <c r="D92" s="44">
+        <f>D94</f>
         <v>2100</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C93" s="2">
         <f t="shared" si="10"/>
         <v>90</v>
       </c>
       <c r="D93" s="44">
+        <f>D94</f>
         <v>2100</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C94" s="2">
         <f t="shared" si="10"/>
         <v>100</v>
@@ -15510,19 +16616,19 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D95" s="45"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C97" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D97" s="52" t="str">
+      <c r="D97" s="48" t="str">
         <f>"{"&amp;ROUND(D84,0)&amp;", "&amp;ROUND(D85,0)&amp;", "&amp;ROUND(D86,0)&amp;", "&amp;ROUND(D87,0)&amp;", "&amp;ROUND(D88,0)&amp;", "&amp;ROUND(D89,0)&amp;", "&amp;ROUND(D90,0)&amp;", "&amp;ROUND(D91,0)&amp;", "&amp;ROUND(D92,0)&amp;", "&amp;ROUND(D93,0)&amp;", "&amp;ROUND(D94,0)&amp;"}"</f>
         <v>{900, 900, 900, 1140, 1380, 1620, 1860, 2100, 2100, 2100, 2100}</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A100">
         <v>6</v>
       </c>
@@ -15530,7 +16636,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C101" s="2" t="s">
         <v>54</v>
       </c>
@@ -15538,7 +16644,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C102" s="2">
         <v>0</v>
       </c>
@@ -15547,7 +16653,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C103" s="2">
         <f>C102+10</f>
         <v>10</v>
@@ -15556,7 +16662,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C104" s="2">
         <f t="shared" ref="C104:C112" si="12">C103+10</f>
         <v>20</v>
@@ -15565,7 +16671,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C105" s="2">
         <f t="shared" si="12"/>
         <v>30</v>
@@ -15574,7 +16680,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C106" s="2">
         <f t="shared" si="12"/>
         <v>40</v>
@@ -15583,7 +16689,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C107" s="2">
         <f t="shared" si="12"/>
         <v>50</v>
@@ -15592,7 +16698,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C108" s="2">
         <f t="shared" si="12"/>
         <v>60</v>
@@ -15601,7 +16707,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C109" s="2">
         <f t="shared" si="12"/>
         <v>70</v>
@@ -15610,7 +16716,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C110" s="2">
         <f t="shared" si="12"/>
         <v>80</v>
@@ -15619,7 +16725,7 @@
         <v>1940</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C111" s="2">
         <f t="shared" si="12"/>
         <v>90</v>
@@ -15628,7 +16734,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C112" s="2">
         <f t="shared" si="12"/>
         <v>100</v>
@@ -15638,16 +16744,16 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C115" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D115" s="52" t="str">
+      <c r="D115" s="48" t="str">
         <f>"{"&amp;ROUND(D102,0)&amp;", "&amp;ROUND(D103,0)&amp;", "&amp;ROUND(D104,0)&amp;", "&amp;ROUND(D105,0)&amp;", "&amp;ROUND(D106,0)&amp;", "&amp;ROUND(D107,0)&amp;", "&amp;ROUND(D108,0)&amp;", "&amp;ROUND(D109,0)&amp;", "&amp;ROUND(D110,0)&amp;", "&amp;ROUND(D111,0)&amp;", "&amp;ROUND(D112,0)&amp;"}"</f>
         <v>{900, 1200, 1350, 1400, 1420, 1480, 1600, 1750, 1940, 2060, 2100}</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A119">
         <v>7</v>
       </c>
@@ -15655,7 +16761,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C120" s="2" t="s">
         <v>54</v>
       </c>
@@ -15663,7 +16769,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C121" s="2">
         <v>0</v>
       </c>
@@ -15672,7 +16778,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C122" s="2">
         <f>C121+10</f>
         <v>10</v>
@@ -15681,7 +16787,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C123" s="2">
         <f t="shared" ref="C123:C131" si="13">C122+10</f>
         <v>20</v>
@@ -15690,7 +16796,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C124" s="2">
         <f t="shared" si="13"/>
         <v>30</v>
@@ -15699,7 +16805,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C125" s="2">
         <f t="shared" si="13"/>
         <v>40</v>
@@ -15708,7 +16814,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C126" s="2">
         <f t="shared" si="13"/>
         <v>50</v>
@@ -15717,7 +16823,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C127" s="2">
         <f t="shared" si="13"/>
         <v>60</v>
@@ -15726,7 +16832,7 @@
         <v>1620</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C128" s="2">
         <f t="shared" si="13"/>
         <v>70</v>
@@ -15735,7 +16841,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C129" s="2">
         <f t="shared" si="13"/>
         <v>80</v>
@@ -15744,7 +16850,7 @@
         <v>1940</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C130" s="2">
         <f t="shared" si="13"/>
         <v>90</v>
@@ -15753,7 +16859,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C131" s="2">
         <f t="shared" si="13"/>
         <v>100</v>
@@ -15763,16 +16869,16 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C134" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D134" s="52" t="str">
+      <c r="D134" s="48" t="str">
         <f>"{"&amp;ROUND(D121,0)&amp;", "&amp;ROUND(D122,0)&amp;", "&amp;ROUND(D123,0)&amp;", "&amp;ROUND(D124,0)&amp;", "&amp;ROUND(D125,0)&amp;", "&amp;ROUND(D126,0)&amp;", "&amp;ROUND(D127,0)&amp;", "&amp;ROUND(D128,0)&amp;", "&amp;ROUND(D129,0)&amp;", "&amp;ROUND(D130,0)&amp;", "&amp;ROUND(D131,0)&amp;"}"</f>
         <v>{900, 1250, 1450, 1550, 1600, 1600, 1620, 1750, 1940, 2060, 2100}</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A137">
         <v>8</v>
       </c>
@@ -15780,7 +16886,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C138" s="2" t="s">
         <v>54</v>
       </c>
@@ -15788,7 +16894,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C139" s="2">
         <v>0</v>
       </c>
@@ -15797,7 +16903,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C140" s="2">
         <f>C139+10</f>
         <v>10</v>
@@ -15806,7 +16912,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C141" s="2">
         <f t="shared" ref="C141:C149" si="14">C140+10</f>
         <v>20</v>
@@ -15815,7 +16921,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C142" s="2">
         <f t="shared" si="14"/>
         <v>30</v>
@@ -15824,7 +16930,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C143" s="2">
         <f t="shared" si="14"/>
         <v>40</v>
@@ -15833,7 +16939,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C144" s="2">
         <f t="shared" si="14"/>
         <v>50</v>
@@ -15842,7 +16948,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C145" s="2">
         <f t="shared" si="14"/>
         <v>60</v>
@@ -15851,7 +16957,7 @@
         <v>1790</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C146" s="2">
         <f t="shared" si="14"/>
         <v>70</v>
@@ -15860,7 +16966,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C147" s="2">
         <f t="shared" si="14"/>
         <v>80</v>
@@ -15869,7 +16975,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C148" s="2">
         <f t="shared" si="14"/>
         <v>90</v>
@@ -15878,7 +16984,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C149" s="2">
         <f t="shared" si="14"/>
         <v>100</v>
@@ -15888,16 +16994,16 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C152" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D152" s="52" t="str">
+      <c r="D152" s="48" t="str">
         <f>"{"&amp;ROUND(D139,0)&amp;", "&amp;ROUND(D140,0)&amp;", "&amp;ROUND(D141,0)&amp;", "&amp;ROUND(D142,0)&amp;", "&amp;ROUND(D143,0)&amp;", "&amp;ROUND(D144,0)&amp;", "&amp;ROUND(D145,0)&amp;", "&amp;ROUND(D146,0)&amp;", "&amp;ROUND(D147,0)&amp;", "&amp;ROUND(D148,0)&amp;", "&amp;ROUND(D149,0)&amp;"}"</f>
         <v>{900, 910, 930, 1020, 1200, 1570, 1790, 1900, 2000, 2070, 2100}</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A155">
         <v>9</v>
       </c>
@@ -15905,7 +17011,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C156" s="2" t="s">
         <v>54</v>
       </c>
@@ -15913,7 +17019,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C157" s="2">
         <v>0</v>
       </c>
@@ -15922,7 +17028,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C158" s="2">
         <f>C157+10</f>
         <v>10</v>
@@ -15931,7 +17037,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C159" s="2">
         <f t="shared" ref="C159:C167" si="15">C158+10</f>
         <v>20</v>
@@ -15940,7 +17046,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C160" s="2">
         <f t="shared" si="15"/>
         <v>30</v>
@@ -15949,7 +17055,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C161" s="2">
         <f t="shared" si="15"/>
         <v>40</v>
@@ -15958,7 +17064,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C162" s="2">
         <f t="shared" si="15"/>
         <v>50</v>
@@ -15967,7 +17073,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C163" s="2">
         <f t="shared" si="15"/>
         <v>60</v>
@@ -15976,7 +17082,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C164" s="2">
         <f t="shared" si="15"/>
         <v>70</v>
@@ -15985,7 +17091,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C165" s="2">
         <f t="shared" si="15"/>
         <v>80</v>
@@ -15994,7 +17100,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C166" s="2">
         <f t="shared" si="15"/>
         <v>90</v>
@@ -16003,7 +17109,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C167" s="2">
         <f t="shared" si="15"/>
         <v>100</v>
@@ -16013,16 +17119,16 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C170" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D170" s="52" t="str">
+      <c r="D170" s="48" t="str">
         <f>"{"&amp;ROUND(D157,0)&amp;", "&amp;ROUND(D158,0)&amp;", "&amp;ROUND(D159,0)&amp;", "&amp;ROUND(D160,0)&amp;", "&amp;ROUND(D161,0)&amp;", "&amp;ROUND(D162,0)&amp;", "&amp;ROUND(D163,0)&amp;", "&amp;ROUND(D164,0)&amp;", "&amp;ROUND(D165,0)&amp;", "&amp;ROUND(D166,0)&amp;", "&amp;ROUND(D167,0)&amp;"}"</f>
         <v>{900, 900, 920, 980, 1200, 1640, 1900, 2010, 2080, 2100, 2100}</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A173">
         <v>10</v>
       </c>
@@ -16030,7 +17136,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C174" s="2" t="s">
         <v>54</v>
       </c>
@@ -16038,7 +17144,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C175" s="2">
         <v>0</v>
       </c>
@@ -16047,7 +17153,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C176" s="2">
         <f>C175+10</f>
         <v>10</v>
@@ -16056,7 +17162,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C177" s="2">
         <f t="shared" ref="C177:C185" si="16">C176+10</f>
         <v>20</v>
@@ -16065,7 +17171,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C178" s="2">
         <f t="shared" si="16"/>
         <v>30</v>
@@ -16074,7 +17180,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C179" s="2">
         <f t="shared" si="16"/>
         <v>40</v>
@@ -16083,7 +17189,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C180" s="2">
         <f t="shared" si="16"/>
         <v>50</v>
@@ -16092,7 +17198,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C181" s="2">
         <f t="shared" si="16"/>
         <v>60</v>
@@ -16101,7 +17207,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C182" s="2">
         <f t="shared" si="16"/>
         <v>70</v>
@@ -16110,7 +17216,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C183" s="2">
         <f t="shared" si="16"/>
         <v>80</v>
@@ -16119,7 +17225,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C184" s="2">
         <f t="shared" si="16"/>
         <v>90</v>
@@ -16128,7 +17234,7 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C185" s="2">
         <f t="shared" si="16"/>
         <v>100</v>
@@ -16138,16 +17244,16 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C188" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D188" s="52" t="str">
+      <c r="D188" s="48" t="str">
         <f>"{"&amp;ROUND(D175,0)&amp;", "&amp;ROUND(D176,0)&amp;", "&amp;ROUND(D177,0)&amp;", "&amp;ROUND(D178,0)&amp;", "&amp;ROUND(D179,0)&amp;", "&amp;ROUND(D180,0)&amp;", "&amp;ROUND(D181,0)&amp;", "&amp;ROUND(D182,0)&amp;", "&amp;ROUND(D183,0)&amp;", "&amp;ROUND(D184,0)&amp;", "&amp;ROUND(D185,0)&amp;"}"</f>
         <v>{900, 900, 910, 930, 990, 1110, 1310, 1590, 1890, 2090, 2100}</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A191">
         <v>11</v>
       </c>
@@ -16155,7 +17261,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C192" s="2" t="s">
         <v>54</v>
       </c>
@@ -16163,7 +17269,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="193" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C193" s="2">
         <v>0</v>
       </c>
@@ -16172,7 +17278,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="194" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C194" s="2">
         <f>C193+10</f>
         <v>10</v>
@@ -16181,7 +17287,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="195" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C195" s="2">
         <f t="shared" ref="C195:C203" si="17">C194+10</f>
         <v>20</v>
@@ -16190,7 +17296,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="196" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C196" s="2">
         <f t="shared" si="17"/>
         <v>30</v>
@@ -16199,7 +17305,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="197" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C197" s="2">
         <f t="shared" si="17"/>
         <v>40</v>
@@ -16208,7 +17314,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="198" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C198" s="2">
         <f t="shared" si="17"/>
         <v>50</v>
@@ -16217,7 +17323,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="199" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C199" s="2">
         <f t="shared" si="17"/>
         <v>60</v>
@@ -16226,7 +17332,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="200" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C200" s="2">
         <f t="shared" si="17"/>
         <v>70</v>
@@ -16235,7 +17341,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="201" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C201" s="2">
         <f t="shared" si="17"/>
         <v>80</v>
@@ -16244,7 +17350,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="202" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C202" s="2">
         <f t="shared" si="17"/>
         <v>90</v>
@@ -16253,7 +17359,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="203" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C203" s="2">
         <f t="shared" si="17"/>
         <v>100</v>
@@ -16263,16 +17369,16 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="206" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C206" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D206" s="52" t="str">
+      <c r="D206" s="48" t="str">
         <f>"{"&amp;ROUND(D193,0)&amp;", "&amp;ROUND(D194,0)&amp;", "&amp;ROUND(D195,0)&amp;", "&amp;ROUND(D196,0)&amp;", "&amp;ROUND(D197,0)&amp;", "&amp;ROUND(D198,0)&amp;", "&amp;ROUND(D199,0)&amp;", "&amp;ROUND(D200,0)&amp;", "&amp;ROUND(D201,0)&amp;", "&amp;ROUND(D202,0)&amp;", "&amp;ROUND(D203,0)&amp;"}"</f>
         <v>{900, 900, 910, 920, 930, 980, 1100, 1300, 1550, 1800, 2100}</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A209">
         <v>12</v>
       </c>
@@ -16280,7 +17386,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C210" s="2" t="s">
         <v>54</v>
       </c>
@@ -16288,7 +17394,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C211" s="2">
         <v>0</v>
       </c>
@@ -16297,7 +17403,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C212" s="2">
         <f>C211+10</f>
         <v>10</v>
@@ -16306,7 +17412,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C213" s="2">
         <f t="shared" ref="C213:C221" si="18">C212+10</f>
         <v>20</v>
@@ -16315,7 +17421,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C214" s="2">
         <f t="shared" si="18"/>
         <v>30</v>
@@ -16324,7 +17430,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C215" s="2">
         <f t="shared" si="18"/>
         <v>40</v>
@@ -16333,7 +17439,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C216" s="2">
         <f t="shared" si="18"/>
         <v>50</v>
@@ -16342,7 +17448,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C217" s="2">
         <f t="shared" si="18"/>
         <v>60</v>
@@ -16351,7 +17457,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C218" s="2">
         <f t="shared" si="18"/>
         <v>70</v>
@@ -16360,7 +17466,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C219" s="2">
         <f t="shared" si="18"/>
         <v>80</v>
@@ -16369,7 +17475,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C220" s="2">
         <f t="shared" si="18"/>
         <v>90</v>
@@ -16378,7 +17484,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C221" s="2">
         <f t="shared" si="18"/>
         <v>100</v>
@@ -16388,13 +17494,179 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C224" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D224" s="52" t="str">
+      <c r="D224" s="48" t="str">
         <f>"{"&amp;ROUND(D211,0)&amp;", "&amp;ROUND(D212,0)&amp;", "&amp;ROUND(D213,0)&amp;", "&amp;ROUND(D214,0)&amp;", "&amp;ROUND(D215,0)&amp;", "&amp;ROUND(D216,0)&amp;", "&amp;ROUND(D217,0)&amp;", "&amp;ROUND(D218,0)&amp;", "&amp;ROUND(D219,0)&amp;", "&amp;ROUND(D220,0)&amp;", "&amp;ROUND(D221,0)&amp;"}"</f>
         <v>{900, 1020, 1140, 1260, 1380, 1380, 1380, 1380, 1650, 1900, 2100}</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A229">
+        <v>13</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E229" s="41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C230" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D230" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E230" s="49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C231" s="2">
+        <v>0</v>
+      </c>
+      <c r="D231" s="44">
+        <f>$B$2</f>
+        <v>900</v>
+      </c>
+      <c r="E231" s="43">
+        <f>C236</f>
+        <v>50</v>
+      </c>
+      <c r="F231" s="46">
+        <f>D236</f>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C232" s="2">
+        <f>C231+10</f>
+        <v>10</v>
+      </c>
+      <c r="D232" s="44">
+        <f>C232*$E$233+$F$233</f>
+        <v>940</v>
+      </c>
+      <c r="E232" s="43">
+        <f>C231</f>
+        <v>0</v>
+      </c>
+      <c r="F232" s="46">
+        <f>D231</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C233" s="2">
+        <f t="shared" ref="C233:C241" si="19">C232+10</f>
+        <v>20</v>
+      </c>
+      <c r="D233" s="44">
+        <f t="shared" ref="D233:D235" si="20">C233*$E$233+$F$233</f>
+        <v>980</v>
+      </c>
+      <c r="E233" s="47">
+        <f>SLOPE(F231:F232,E231:E232)</f>
+        <v>4</v>
+      </c>
+      <c r="F233" s="43">
+        <f>INTERCEPT(F231:F232,E231:E232)</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C234" s="2">
+        <f t="shared" si="19"/>
+        <v>30</v>
+      </c>
+      <c r="D234" s="44">
+        <f t="shared" si="20"/>
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C235" s="2">
+        <f t="shared" si="19"/>
+        <v>40</v>
+      </c>
+      <c r="D235" s="44">
+        <f t="shared" si="20"/>
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C236" s="2">
+        <f t="shared" si="19"/>
+        <v>50</v>
+      </c>
+      <c r="D236" s="44">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C237" s="2">
+        <f t="shared" si="19"/>
+        <v>60</v>
+      </c>
+      <c r="D237" s="44">
+        <f>$C237*$E$230 +$D$236</f>
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C238" s="2">
+        <f t="shared" si="19"/>
+        <v>70</v>
+      </c>
+      <c r="D238" s="44">
+        <f t="shared" ref="D238:D240" si="21">$C238*$E$230 +$D$236</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C239" s="2">
+        <f t="shared" si="19"/>
+        <v>80</v>
+      </c>
+      <c r="D239" s="44">
+        <f t="shared" si="21"/>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C240" s="2">
+        <f t="shared" si="19"/>
+        <v>90</v>
+      </c>
+      <c r="D240" s="44">
+        <f t="shared" si="21"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="241" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C241" s="2">
+        <f t="shared" si="19"/>
+        <v>100</v>
+      </c>
+      <c r="D241" s="44">
+        <f>$C$2</f>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="244" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C244" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D244" s="48" t="str">
+        <f>"{"&amp;ROUND(D231,0)&amp;", "&amp;ROUND(D232,0)&amp;", "&amp;ROUND(D233,0)&amp;", "&amp;ROUND(D234,0)&amp;", "&amp;ROUND(D235,0)&amp;", "&amp;ROUND(D236,0)&amp;", "&amp;ROUND(D237,0)&amp;", "&amp;ROUND(D238,0)&amp;", "&amp;ROUND(D239,0)&amp;", "&amp;ROUND(D240,0)&amp;", "&amp;ROUND(D241,0)&amp;"}"</f>
+        <v>{900, 940, 980, 1020, 1060, 1100, 1700, 1800, 1900, 2000, 2100}</v>
       </c>
     </row>
   </sheetData>
@@ -16409,7 +17681,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16421,7 +17693,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16433,7 +17705,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ClutchPaddleMaps & Minor Changes
updated the first 11 clutch maps
</commit_message>
<xml_diff>
--- a/Docs/P19_Maps_v01.xlsx
+++ b/Docs/P19_Maps_v01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03.CODE\P19-Shifter\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1817B12D-E431-4276-B6D2-916C479ABF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60BB628-6D53-4A42-8580-FC2D13AB4852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{B721293F-9984-497B-84C2-5BF522F68054}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{B721293F-9984-497B-84C2-5BF522F68054}"/>
   </bookViews>
   <sheets>
     <sheet name="TODOs" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -221,25 +221,7 @@
     <t>Progressive 3</t>
   </si>
   <si>
-    <t>Hill 1</t>
-  </si>
-  <si>
-    <t>Hill 2</t>
-  </si>
-  <si>
-    <t>Y 1</t>
-  </si>
-  <si>
-    <t>Y 2</t>
-  </si>
-  <si>
     <t>Start 1</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>S 2</t>
   </si>
   <si>
     <t>Map to copy:</t>
@@ -287,9 +269,6 @@
     <t>BitePoint 1</t>
   </si>
   <si>
-    <t>make more maps like this and change the gain</t>
-  </si>
-  <si>
     <t>map the rotary with the various voltages</t>
   </si>
   <si>
@@ -321,6 +300,45 @@
   </si>
   <si>
     <t>Shifting tests</t>
+  </si>
+  <si>
+    <t>BitePoint 2</t>
+  </si>
+  <si>
+    <t>BitePoint 3</t>
+  </si>
+  <si>
+    <t>BitePoint 4</t>
+  </si>
+  <si>
+    <t>@10</t>
+  </si>
+  <si>
+    <t>@20</t>
+  </si>
+  <si>
+    <t>@30</t>
+  </si>
+  <si>
+    <t>@40</t>
+  </si>
+  <si>
+    <t>S 1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>@60%</t>
+  </si>
+  <si>
+    <t>@50%</t>
+  </si>
+  <si>
+    <t>@40%</t>
   </si>
 </sst>
 </file>
@@ -400,7 +418,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,6 +440,66 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -723,7 +801,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -867,6 +945,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -882,7 +961,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1487,7 +1604,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$C$175:$C$185</c:f>
+              <c:f>ClutchPaddle!$C$173:$C$183</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1529,7 +1646,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$D$175:$D$185</c:f>
+              <c:f>ClutchPaddle!$D$173:$D$183</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1537,31 +1654,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>900</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>910</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>930</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>990</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1110</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1310</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1590</c:v>
+                  <c:v>4.55</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1890</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2090</c:v>
+                  <c:v>4.95</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>5</c:v>
@@ -1972,7 +2089,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$C$193:$C$203</c:f>
+              <c:f>ClutchPaddle!$C$191:$C$201</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2014,7 +2131,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$D$193:$D$203</c:f>
+              <c:f>ClutchPaddle!$D$191:$D$201</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2022,31 +2139,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>900</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>910</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>920</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>930</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>980</c:v>
+                  <c:v>3.65</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1100</c:v>
+                  <c:v>4.3499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1300</c:v>
+                  <c:v>4.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1550</c:v>
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1800</c:v>
+                  <c:v>4.95</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>5</c:v>
@@ -2457,7 +2574,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$C$211:$C$221</c:f>
+              <c:f>ClutchPaddle!$C$209:$C$219</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2499,7 +2616,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$D$211:$D$221</c:f>
+              <c:f>ClutchPaddle!$D$209:$D$219</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2680,7 +2797,7 @@
         <c:axId val="1955299072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="5"/>
+          <c:max val="2100"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2942,7 +3059,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$C$231:$C$241</c:f>
+              <c:f>ClutchPaddle!$C$229:$C$239</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2984,7 +3101,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$D$231:$D$241</c:f>
+              <c:f>ClutchPaddle!$D$229:$D$239</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2992,31 +3109,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>220</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>440</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>660</c:v>
+                  <c:v>1.7999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>880</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1100</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1700</c:v>
+                  <c:v>3.06</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1800</c:v>
+                  <c:v>3.07</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1900</c:v>
+                  <c:v>3.08</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2000</c:v>
+                  <c:v>3.09</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>5</c:v>
@@ -3894,7 +4011,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Map 2</a:t>
+              <a:t> Map 6</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -3952,7 +4069,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$C$26:$C$36</c:f>
+              <c:f>ClutchPaddle!$C$99:$C$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3994,7 +4111,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$D$26:$D$36</c:f>
+              <c:f>ClutchPaddle!$D$99:$D$109</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4374,7 +4491,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Map 3</a:t>
+              <a:t> Map 7</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -4432,7 +4549,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$C$44:$C$54</c:f>
+              <c:f>ClutchPaddle!$C$117:$C$127</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4474,7 +4591,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$D$44:$D$54</c:f>
+              <c:f>ClutchPaddle!$D$117:$D$127</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4854,7 +4971,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Map 4</a:t>
+              <a:t> Map 8</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4911,7 +5028,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$C$64:$C$74</c:f>
+              <c:f>ClutchPaddle!$C$137:$C$147</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4953,7 +5070,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$D$64:$D$74</c:f>
+              <c:f>ClutchPaddle!$D$137:$D$147</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5333,7 +5450,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Map 5</a:t>
+              <a:t> Map 2</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5390,7 +5507,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$C$84:$C$94</c:f>
+              <c:f>ClutchPaddle!$C$25:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5432,7 +5549,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$D$84:$D$94</c:f>
+              <c:f>ClutchPaddle!$D$25:$D$35</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5443,25 +5560,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>1.875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>3.125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>3.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>4.375</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>5</c:v>
@@ -5812,7 +5929,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Map 6</a:t>
+              <a:t> Map 3</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5869,7 +5986,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$C$102:$C$112</c:f>
+              <c:f>ClutchPaddle!$C$43:$C$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5911,7 +6028,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$D$102:$D$112</c:f>
+              <c:f>ClutchPaddle!$D$43:$D$53</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -5919,31 +6036,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1350</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1400</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1420</c:v>
+                  <c:v>1.6666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1480</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1600</c:v>
+                  <c:v>3.3333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1750</c:v>
+                  <c:v>4.166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1940</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2060</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>5</c:v>
@@ -6291,14 +6408,8 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Map 7</a:t>
+              <a:t> Map 4</a:t>
             </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US" baseline="0"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -6354,7 +6465,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$C$121:$C$131</c:f>
+              <c:f>ClutchPaddle!$C$61:$C$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -6396,7 +6507,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$D$121:$D$131</c:f>
+              <c:f>ClutchPaddle!$D$61:$D$71</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -6404,31 +6515,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1250</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1450</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1550</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1600</c:v>
+                  <c:v>1.6666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1600</c:v>
+                  <c:v>3.3333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1620</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1750</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1940</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2060</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>5</c:v>
@@ -6776,14 +6887,8 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Map 8</a:t>
+              <a:t> Map 5</a:t>
             </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US" baseline="0"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -6839,7 +6944,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$C$139:$C$149</c:f>
+              <c:f>ClutchPaddle!$C$79:$C$89</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -6881,7 +6986,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$D$139:$D$149</c:f>
+              <c:f>ClutchPaddle!$D$79:$D$89</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -6889,31 +6994,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>910</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>930</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1020</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1570</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1790</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1900</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2070</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>5</c:v>
@@ -7334,7 +7439,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$C$157:$C$167</c:f>
+              <c:f>ClutchPaddle!$C$155:$C$165</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -7376,7 +7481,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ClutchPaddle!$D$157:$D$167</c:f>
+              <c:f>ClutchPaddle!$D$155:$D$165</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -7384,31 +7489,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>900</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>920</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>980</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1200</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1640</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1900</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2010</c:v>
+                  <c:v>3.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2080</c:v>
+                  <c:v>4.7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2100</c:v>
+                  <c:v>4.95</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>5</c:v>
@@ -15725,15 +15830,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>117156</xdr:rowOff>
+      <xdr:colOff>255270</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>170496</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>7619</xdr:rowOff>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>60959</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15764,13 +15869,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>278130</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>40956</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>434340</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -15802,13 +15907,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>339090</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>134</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>149</xdr:row>
       <xdr:rowOff>83819</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -15839,15 +15944,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>331470</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>124776</xdr:rowOff>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>48576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>487680</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>15239</xdr:rowOff>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>121919</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15877,15 +15982,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>308610</xdr:colOff>
-      <xdr:row>99</xdr:row>
-      <xdr:rowOff>117156</xdr:rowOff>
+      <xdr:colOff>377190</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>33336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>115</xdr:row>
-      <xdr:rowOff>7619</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>106679</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15916,14 +16021,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>18096</xdr:rowOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>63816</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>133</xdr:row>
-      <xdr:rowOff>91439</xdr:rowOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>137159</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15953,15 +16058,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>339090</xdr:colOff>
-      <xdr:row>136</xdr:row>
-      <xdr:rowOff>117156</xdr:rowOff>
+      <xdr:colOff>308610</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>18096</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>152</xdr:row>
-      <xdr:rowOff>7619</xdr:rowOff>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>91439</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15992,13 +16097,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>339090</xdr:colOff>
-      <xdr:row>153</xdr:row>
-      <xdr:rowOff>170496</xdr:rowOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>169</xdr:row>
+      <xdr:row>167</xdr:row>
       <xdr:rowOff>60959</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -16030,13 +16135,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>339090</xdr:colOff>
-      <xdr:row>171</xdr:row>
+      <xdr:row>169</xdr:row>
       <xdr:rowOff>155256</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>187</xdr:row>
+      <xdr:row>185</xdr:row>
       <xdr:rowOff>45719</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -16068,13 +16173,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>189</xdr:row>
+      <xdr:row>187</xdr:row>
       <xdr:rowOff>147636</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>205</xdr:row>
+      <xdr:row>203</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -16106,13 +16211,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>369570</xdr:colOff>
-      <xdr:row>207</xdr:row>
+      <xdr:row>205</xdr:row>
       <xdr:rowOff>162876</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>223</xdr:row>
+      <xdr:row>221</xdr:row>
       <xdr:rowOff>53339</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -16144,13 +16249,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>375012</xdr:colOff>
-      <xdr:row>226</xdr:row>
+      <xdr:row>224</xdr:row>
       <xdr:rowOff>168319</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>531222</xdr:colOff>
-      <xdr:row>242</xdr:row>
+      <xdr:row>240</xdr:row>
       <xdr:rowOff>58781</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -16541,65 +16646,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB42887-2D23-4471-814F-CA0960C53B07}">
   <dimension ref="B3:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="58" t="s">
-        <v>88</v>
+      <c r="B3" s="53" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B12" s="58" t="s">
-        <v>92</v>
+      <c r="B12" s="53" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -16669,7 +16774,7 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="54" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="32" t="s">
@@ -16710,7 +16815,7 @@
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="54"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="32" t="s">
         <v>24</v>
       </c>
@@ -16749,7 +16854,7 @@
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="54"/>
+      <c r="B8" s="55"/>
       <c r="C8" s="32" t="s">
         <v>26</v>
       </c>
@@ -16786,7 +16891,7 @@
       <c r="N8" s="31"/>
     </row>
     <row r="9" spans="2:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="55"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="32" t="s">
         <v>51</v>
       </c>
@@ -17100,10 +17205,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327977B7-E239-49BB-B0DD-EEBF381339C3}">
-  <dimension ref="A1:P244"/>
+  <dimension ref="A1:F242"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView tabSelected="1" topLeftCell="A191" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R206" sqref="R206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17117,15 +17222,15 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="41" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B2" s="42">
         <v>0</v>
@@ -17138,7 +17243,7 @@
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="60" t="s">
         <v>55</v>
       </c>
     </row>
@@ -17147,7 +17252,7 @@
         <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -17268,1699 +17373,1761 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C20" s="40" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D20" s="51" t="str">
         <f>"{"&amp;TEXT(ROUND(D7,2),"0.00")&amp;", "&amp;TEXT(ROUND(D8,2),"0.00")&amp;", "&amp;TEXT(ROUND(D9,2),"0.00")&amp;", "&amp;TEXT(ROUND(D10,2),"0.00")&amp;", "&amp;TEXT(ROUND(D11,2),"0.00")&amp;", "&amp;TEXT(ROUND(D12,2),"0.00")&amp;", "&amp;TEXT(ROUND(D13,2),"0.00")&amp;", "&amp;TEXT(ROUND(D14,2),"0.00")&amp;", "&amp;TEXT(ROUND(D15,2),"0.00")&amp;", "&amp;TEXT(ROUND(D16,2),"0.00")&amp;", "&amp;TEXT(ROUND(D17,2),"0.00")&amp;"}"</f>
         <v>{0.00, 0.50, 1.00, 1.50, 2.00, 2.50, 3.00, 3.50, 4.00, 4.50, 5.00}</v>
       </c>
     </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="64" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>2</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="41" t="s">
-        <v>70</v>
+        <v>54</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C25" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" s="47">
-        <v>0.1</v>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="49">
+        <f>$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="48">
+        <f>(D34-D26)/8</f>
+        <v>0.625</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C26" s="2">
+        <f>C25+10</f>
+        <v>10</v>
+      </c>
+      <c r="D26" s="49">
+        <f>D25</f>
         <v>0</v>
-      </c>
-      <c r="D26" s="49">
-        <f>$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="43">
-        <f>C30</f>
-        <v>40</v>
-      </c>
-      <c r="F26" s="45">
-        <f>D30</f>
-        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C27" s="2">
-        <f>C26+10</f>
-        <v>10</v>
+        <f t="shared" ref="C27:C35" si="2">C26+10</f>
+        <v>20</v>
       </c>
       <c r="D27" s="49">
-        <f>C27*$E$25+$D$26</f>
-        <v>1</v>
-      </c>
-      <c r="E27" s="43">
-        <f>C36</f>
-        <v>100</v>
-      </c>
-      <c r="F27" s="43">
-        <f>D36</f>
-        <v>5</v>
+        <f>D26+$E$25</f>
+        <v>0.625</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C28" s="2">
-        <f t="shared" ref="C28:C36" si="2">C27+10</f>
-        <v>20</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="D28" s="49">
-        <f t="shared" ref="D28:D30" si="3">C28*$E$25+$D$26</f>
-        <v>2</v>
-      </c>
-      <c r="E28" s="46">
-        <f>SLOPE(F26:F27,E26:E27)</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-      <c r="F28" s="43">
-        <f>INTERCEPT(F26:F27,E26:E27)</f>
-        <v>3.333333333333333</v>
+        <f>D27+$E$25</f>
+        <v>1.25</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C29" s="2">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D29" s="49">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f>D28+$E$25</f>
+        <v>1.875</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C30" s="2">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D30" s="49">
-        <f t="shared" si="3"/>
-        <v>4</v>
+        <f>D29+$E$25</f>
+        <v>2.5</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C31" s="2">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D31" s="49">
-        <f>C31*$E$28+$F$28</f>
-        <v>4.1666666666666661</v>
+        <f>D30+$E$25</f>
+        <v>3.125</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C32" s="2">
         <f t="shared" si="2"/>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D32" s="49">
-        <f t="shared" ref="D32:D35" si="4">C32*$E$28+$F$28</f>
-        <v>4.333333333333333</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <f>D31+$E$25</f>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C33" s="2">
         <f t="shared" si="2"/>
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D33" s="49">
-        <f t="shared" si="4"/>
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <f>D32+$E$25</f>
+        <v>4.375</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C34" s="2">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D34" s="49">
-        <f t="shared" si="4"/>
-        <v>4.6666666666666661</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <f>D35</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C35" s="2">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D35" s="49">
-        <f t="shared" si="4"/>
-        <v>4.833333333333333</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C36" s="2">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="D36" s="49">
         <f>$C$2</f>
         <v>5</v>
       </c>
-      <c r="F36" s="50"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C39" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D39" s="51" t="str">
-        <f>"{"&amp;TEXT(ROUND(D26,2),"0.00")&amp;", "&amp;TEXT(ROUND(D27,2),"0.00")&amp;", "&amp;TEXT(ROUND(D28,2),"0.00")&amp;", "&amp;TEXT(ROUND(D29,2),"0.00")&amp;", "&amp;TEXT(ROUND(D30,2),"0.00")&amp;", "&amp;TEXT(ROUND(D31,2),"0.00")&amp;", "&amp;TEXT(ROUND(D32,2),"0.00")&amp;", "&amp;TEXT(ROUND(D33,2),"0.00")&amp;", "&amp;TEXT(ROUND(D34,2),"0.00")&amp;", "&amp;TEXT(ROUND(D35,2),"0.00")&amp;", "&amp;TEXT(ROUND(D36,2),"0.00")&amp;"}"</f>
-        <v>{0.00, 1.00, 2.00, 3.00, 4.00, 4.17, 4.33, 4.50, 4.67, 4.83, 5.00}</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D36" s="44"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C38" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="51" t="str">
+        <f>"{"&amp;TEXT(ROUND(D25,2),"0.00")&amp;", "&amp;TEXT(ROUND(D26,2),"0.00")&amp;", "&amp;TEXT(ROUND(D27,2),"0.00")&amp;", "&amp;TEXT(ROUND(D28,2),"0.00")&amp;", "&amp;TEXT(ROUND(D29,2),"0.00")&amp;", "&amp;TEXT(ROUND(D30,2),"0.00")&amp;", "&amp;TEXT(ROUND(D31,2),"0.00")&amp;", "&amp;TEXT(ROUND(D32,2),"0.00")&amp;", "&amp;TEXT(ROUND(D33,2),"0.00")&amp;", "&amp;TEXT(ROUND(D34,2),"0.00")&amp;", "&amp;TEXT(ROUND(D35,2),"0.00")&amp;"}"</f>
+        <v>{0.00, 0.00, 0.63, 1.25, 1.88, 2.50, 3.13, 3.75, 4.38, 5.00, 5.00}</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
         <v>3</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="B41" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C42" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E42" s="41" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C43" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" s="47">
-        <v>0.1333</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C44" s="2">
+      <c r="D42" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C43" s="2">
         <v>0</v>
       </c>
-      <c r="D44" s="49">
+      <c r="D43" s="49">
         <f>$B$2</f>
         <v>0</v>
       </c>
-      <c r="E44" s="43">
-        <f>C47</f>
+      <c r="E43" s="48">
+        <f>(D51-D45)/6</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C44" s="2">
+        <f>C43+10</f>
+        <v>10</v>
+      </c>
+      <c r="D44" s="49">
+        <f>D43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C45" s="2">
+        <f t="shared" ref="C45:C53" si="3">C44+10</f>
+        <v>20</v>
+      </c>
+      <c r="D45" s="49">
+        <f>D44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C46" s="2">
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="F44" s="45">
-        <f>D47</f>
-        <v>3.9990000000000001</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C45" s="2">
-        <f>C44+10</f>
+      <c r="D46" s="49">
+        <f>D45+$E$43</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C47" s="2">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="D47" s="49">
+        <f>D46+$E$43</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C48" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="D48" s="49">
+        <f>D47+$E$43</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C49" s="2">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="D49" s="49">
+        <f>D48+$E$43</f>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C50" s="2">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="D50" s="49">
+        <f>D49+$E$43</f>
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C51" s="2">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="D51" s="49">
+        <f>D53</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C52" s="2">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="D52" s="49">
+        <f>D53</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C53" s="2">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="D53" s="49">
+        <f>$C$2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C56" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D56" s="51" t="str">
+        <f>"{"&amp;TEXT(ROUND(D43,2),"0.00")&amp;", "&amp;TEXT(ROUND(D44,2),"0.00")&amp;", "&amp;TEXT(ROUND(D45,2),"0.00")&amp;", "&amp;TEXT(ROUND(D46,2),"0.00")&amp;", "&amp;TEXT(ROUND(D47,2),"0.00")&amp;", "&amp;TEXT(ROUND(D48,2),"0.00")&amp;", "&amp;TEXT(ROUND(D49,2),"0.00")&amp;", "&amp;TEXT(ROUND(D50,2),"0.00")&amp;", "&amp;TEXT(ROUND(D51,2),"0.00")&amp;", "&amp;TEXT(ROUND(D52,2),"0.00")&amp;", "&amp;TEXT(ROUND(D53,2),"0.00")&amp;"}"</f>
+        <v>{0.00, 0.00, 0.00, 0.83, 1.67, 2.50, 3.33, 4.17, 5.00, 5.00, 5.00}</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>4</v>
+      </c>
+      <c r="B59" s="62" t="s">
+        <v>87</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C60" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C61" s="2">
+        <v>0</v>
+      </c>
+      <c r="D61" s="49">
+        <f>$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="E61" s="48">
+        <f>(D68-D64)/3</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C62" s="2">
+        <f>C61+10</f>
         <v>10</v>
       </c>
-      <c r="D45" s="49">
-        <f>C45*$E$43+$D$44</f>
-        <v>1.333</v>
-      </c>
-      <c r="E45" s="43">
-        <f>C54</f>
+      <c r="D62" s="49">
+        <f>D61</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C63" s="2">
+        <f t="shared" ref="C63:C71" si="4">C62+10</f>
+        <v>20</v>
+      </c>
+      <c r="D63" s="49">
+        <f>D62</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C64" s="2">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D64" s="49">
+        <f>D61</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C65" s="2">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D65" s="49">
+        <f>D64+$E$61</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C66" s="2">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="D66" s="49">
+        <f>D65+$E$61</f>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C67" s="2">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="D67" s="49">
+        <f>D66+$E$61</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C68" s="2">
+        <f t="shared" si="4"/>
+        <v>70</v>
+      </c>
+      <c r="D68" s="49">
+        <f>D71</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C69" s="2">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+      <c r="D69" s="49">
+        <f>D71</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C70" s="2">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="D70" s="49">
+        <f>D71</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C71" s="2">
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="F45" s="43">
-        <f>D54</f>
+      <c r="D71" s="49">
+        <f>$C$2</f>
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C46" s="2">
-        <f t="shared" ref="C46:C54" si="5">C45+10</f>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C74" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D74" s="51" t="str">
+        <f>"{"&amp;TEXT(ROUND(D61,2),"0.00")&amp;", "&amp;TEXT(ROUND(D62,2),"0.00")&amp;", "&amp;TEXT(ROUND(D63,2),"0.00")&amp;", "&amp;TEXT(ROUND(D64,2),"0.00")&amp;", "&amp;TEXT(ROUND(D65,2),"0.00")&amp;", "&amp;TEXT(ROUND(D66,2),"0.00")&amp;", "&amp;TEXT(ROUND(D67,2),"0.00")&amp;", "&amp;TEXT(ROUND(D68,2),"0.00")&amp;", "&amp;TEXT(ROUND(D69,2),"0.00")&amp;", "&amp;TEXT(ROUND(D70,2),"0.00")&amp;", "&amp;TEXT(ROUND(D71,2),"0.00")&amp;"}"</f>
+        <v>{0.00, 0.00, 0.00, 0.00, 1.67, 3.33, 5.00, 5.00, 5.00, 5.00, 5.00}</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>5</v>
+      </c>
+      <c r="B77" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C78" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C79" s="2">
+        <v>0</v>
+      </c>
+      <c r="D79" s="49">
+        <f>$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="E79" s="48">
+        <f>(D85-D83)/1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C80" s="2">
+        <f>C79+10</f>
+        <v>10</v>
+      </c>
+      <c r="D80" s="49">
+        <f>D79</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C81" s="2">
+        <f t="shared" ref="C81:C89" si="5">C80+10</f>
         <v>20</v>
       </c>
-      <c r="D46" s="49">
-        <f t="shared" ref="D46:D47" si="6">C46*$E$43+$D$44</f>
-        <v>2.6659999999999999</v>
-      </c>
-      <c r="E46" s="46">
-        <f>SLOPE(F44:F45,E44:E45)</f>
-        <v>1.4299999999999998E-2</v>
-      </c>
-      <c r="F46" s="43">
-        <f>INTERCEPT(F44:F45,E44:E45)</f>
-        <v>3.5700000000000003</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C47" s="2">
+      <c r="D81" s="49">
+        <f>D80</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C82" s="2">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="D47" s="49">
-        <f t="shared" si="6"/>
-        <v>3.9990000000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C48" s="2">
+      <c r="D82" s="49">
+        <f>D79</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C83" s="2">
         <f t="shared" si="5"/>
         <v>40</v>
       </c>
-      <c r="D48" s="49">
-        <f>C48*$E$46+$F$46</f>
-        <v>4.1420000000000003</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C49" s="2">
+      <c r="D83" s="49">
+        <f>D79</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C84" s="2">
         <f t="shared" si="5"/>
         <v>50</v>
       </c>
-      <c r="D49" s="49">
-        <f t="shared" ref="D49:D53" si="7">C49*$E$46+$F$46</f>
-        <v>4.2850000000000001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C50" s="2">
+      <c r="D84" s="49">
+        <f>D83+$E$79</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C85" s="2">
         <f t="shared" si="5"/>
         <v>60</v>
       </c>
-      <c r="D50" s="49">
-        <f t="shared" si="7"/>
-        <v>4.4279999999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C51" s="2">
+      <c r="D85" s="49">
+        <f>D89</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C86" s="2">
         <f t="shared" si="5"/>
         <v>70</v>
       </c>
-      <c r="D51" s="49">
-        <f t="shared" si="7"/>
-        <v>4.5709999999999997</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C52" s="2">
+      <c r="D86" s="49">
+        <f>D89</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C87" s="2">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
-      <c r="D52" s="49">
-        <f t="shared" si="7"/>
-        <v>4.7140000000000004</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C53" s="2">
+      <c r="D87" s="49">
+        <f>D89</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C88" s="2">
         <f t="shared" si="5"/>
         <v>90</v>
       </c>
-      <c r="D53" s="49">
-        <f t="shared" si="7"/>
-        <v>4.8570000000000002</v>
-      </c>
-      <c r="F53" s="50"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C54" s="2">
+      <c r="D88" s="49">
+        <f>D89</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C89" s="2">
         <f t="shared" si="5"/>
         <v>100</v>
       </c>
-      <c r="D54" s="49">
+      <c r="D89" s="49">
         <f>$C$2</f>
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C57" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D57" s="51" t="str">
-        <f>"{"&amp;TEXT(ROUND(D44,2),"0.00")&amp;", "&amp;TEXT(ROUND(D45,2),"0.00")&amp;", "&amp;TEXT(ROUND(D46,2),"0.00")&amp;", "&amp;TEXT(ROUND(D47,2),"0.00")&amp;", "&amp;TEXT(ROUND(D48,2),"0.00")&amp;", "&amp;TEXT(ROUND(D49,2),"0.00")&amp;", "&amp;TEXT(ROUND(D50,2),"0.00")&amp;", "&amp;TEXT(ROUND(D51,2),"0.00")&amp;", "&amp;TEXT(ROUND(D52,2),"0.00")&amp;", "&amp;TEXT(ROUND(D53,2),"0.00")&amp;", "&amp;TEXT(ROUND(D54,2),"0.00")&amp;"}"</f>
-        <v>{0.00, 1.33, 2.67, 4.00, 4.14, 4.29, 4.43, 4.57, 4.71, 4.86, 5.00}</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <v>4</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E62" s="41" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C63" s="2" t="s">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C92" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D92" s="51" t="str">
+        <f>"{"&amp;TEXT(ROUND(D79,2),"0.00")&amp;", "&amp;TEXT(ROUND(D80,2),"0.00")&amp;", "&amp;TEXT(ROUND(D81,2),"0.00")&amp;", "&amp;TEXT(ROUND(D82,2),"0.00")&amp;", "&amp;TEXT(ROUND(D83,2),"0.00")&amp;", "&amp;TEXT(ROUND(D84,2),"0.00")&amp;", "&amp;TEXT(ROUND(D85,2),"0.00")&amp;", "&amp;TEXT(ROUND(D86,2),"0.00")&amp;", "&amp;TEXT(ROUND(D87,2),"0.00")&amp;", "&amp;TEXT(ROUND(D88,2),"0.00")&amp;", "&amp;TEXT(ROUND(D89,2),"0.00")&amp;"}"</f>
+        <v>{0.00, 0.00, 0.00, 0.00, 0.00, 5.00, 5.00, 5.00, 5.00, 5.00, 5.00}</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>6</v>
+      </c>
+      <c r="B97" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E97" s="41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C98" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E63" s="47">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C64" s="2">
+      <c r="D98" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E98" s="47">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C99" s="2">
         <v>0</v>
       </c>
-      <c r="D64" s="49">
+      <c r="D99" s="49">
         <f>$B$2</f>
         <v>0</v>
       </c>
-      <c r="E64" s="43">
-        <f>C66</f>
+      <c r="E99" s="43">
+        <f>C103</f>
+        <v>40</v>
+      </c>
+      <c r="F99" s="45">
+        <f>D103</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C100" s="2">
+        <f>C99+10</f>
+        <v>10</v>
+      </c>
+      <c r="D100" s="49">
+        <f>C100*$E$98+$D$99</f>
+        <v>1</v>
+      </c>
+      <c r="E100" s="43">
+        <f>C109</f>
+        <v>100</v>
+      </c>
+      <c r="F100" s="43">
+        <f>D109</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C101" s="2">
+        <f t="shared" ref="C101:C109" si="6">C100+10</f>
         <v>20</v>
       </c>
-      <c r="F64" s="43">
-        <f>D66</f>
+      <c r="D101" s="49">
+        <f t="shared" ref="D101:D103" si="7">C101*$E$98+$D$99</f>
+        <v>2</v>
+      </c>
+      <c r="E101" s="46">
+        <f>SLOPE(F99:F100,E99:E100)</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F101" s="43">
+        <f>INTERCEPT(F99:F100,E99:E100)</f>
+        <v>3.333333333333333</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C102" s="2">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="D102" s="49">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C103" s="2">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="D103" s="49">
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C65" s="2">
-        <f>C64+10</f>
-        <v>10</v>
-      </c>
-      <c r="D65" s="49">
-        <f>C65*$E$63 +$D$64</f>
-        <v>2</v>
-      </c>
-      <c r="E65" s="43">
-        <f>C74</f>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C104" s="2">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="D104" s="49">
+        <f>C104*$E$101+$F$101</f>
+        <v>4.1666666666666661</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C105" s="2">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+      <c r="D105" s="49">
+        <f t="shared" ref="D105:D108" si="8">C105*$E$101+$F$101</f>
+        <v>4.333333333333333</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C106" s="2">
+        <f t="shared" si="6"/>
+        <v>70</v>
+      </c>
+      <c r="D106" s="49">
+        <f t="shared" si="8"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C107" s="2">
+        <f t="shared" si="6"/>
+        <v>80</v>
+      </c>
+      <c r="D107" s="49">
+        <f t="shared" si="8"/>
+        <v>4.6666666666666661</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C108" s="2">
+        <f t="shared" si="6"/>
+        <v>90</v>
+      </c>
+      <c r="D108" s="49">
+        <f t="shared" si="8"/>
+        <v>4.833333333333333</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C109" s="2">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
-      <c r="F65" s="43">
-        <f>D74</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C66" s="2">
-        <f t="shared" ref="C66:C74" si="8">C65+10</f>
-        <v>20</v>
-      </c>
-      <c r="D66" s="49">
-        <f>C66*$E$63 +$D$64</f>
-        <v>4</v>
-      </c>
-      <c r="E66" s="46">
-        <f>SLOPE(F64:F65,E64:E65)</f>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="F66" s="43">
-        <f>INTERCEPT(F64:F65,E64:E65)</f>
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C67" s="2">
-        <f t="shared" si="8"/>
-        <v>30</v>
-      </c>
-      <c r="D67" s="49">
-        <f>C67*$E$66+$F$66</f>
-        <v>4.125</v>
-      </c>
-    </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C68" s="2">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D68" s="49">
-        <f t="shared" ref="D68:D73" si="9">C68*$E$66+$F$66</f>
-        <v>4.25</v>
-      </c>
-    </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C69" s="2">
-        <f t="shared" si="8"/>
-        <v>50</v>
-      </c>
-      <c r="D69" s="49">
-        <f t="shared" si="9"/>
-        <v>4.375</v>
-      </c>
-    </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C70" s="2">
-        <f t="shared" si="8"/>
-        <v>60</v>
-      </c>
-      <c r="D70" s="49">
-        <f t="shared" si="9"/>
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C71" s="2">
-        <f t="shared" si="8"/>
-        <v>70</v>
-      </c>
-      <c r="D71" s="49">
-        <f t="shared" si="9"/>
-        <v>4.625</v>
-      </c>
-    </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C72" s="2">
-        <f t="shared" si="8"/>
-        <v>80</v>
-      </c>
-      <c r="D72" s="49">
-        <f t="shared" si="9"/>
-        <v>4.75</v>
-      </c>
-    </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C73" s="2">
-        <f t="shared" si="8"/>
-        <v>90</v>
-      </c>
-      <c r="D73" s="49">
-        <f t="shared" si="9"/>
-        <v>4.875</v>
-      </c>
-    </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C74" s="2">
-        <f t="shared" si="8"/>
-        <v>100</v>
-      </c>
-      <c r="D74" s="49">
+      <c r="D109" s="49">
         <f>$C$2</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C77" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D77" s="51" t="str">
-        <f>"{"&amp;TEXT(ROUND(D64,2),"0.00")&amp;", "&amp;TEXT(ROUND(D65,2),"0.00")&amp;", "&amp;TEXT(ROUND(D66,2),"0.00")&amp;", "&amp;TEXT(ROUND(D67,2),"0.00")&amp;", "&amp;TEXT(ROUND(D68,2),"0.00")&amp;", "&amp;TEXT(ROUND(D69,2),"0.00")&amp;", "&amp;TEXT(ROUND(D70,2),"0.00")&amp;", "&amp;TEXT(ROUND(D71,2),"0.00")&amp;", "&amp;TEXT(ROUND(D72,2),"0.00")&amp;", "&amp;TEXT(ROUND(D73,2),"0.00")&amp;", "&amp;TEXT(ROUND(D74,2),"0.00")&amp;"}"</f>
-        <v>{0.00, 2.00, 4.00, 4.13, 4.25, 4.38, 4.50, 4.63, 4.75, 4.88, 5.00}</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A82">
-        <v>5</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C83" s="2" t="s">
+      <c r="F109" s="50"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C112" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D112" s="51" t="str">
+        <f>"{"&amp;TEXT(ROUND(D99,2),"0.00")&amp;", "&amp;TEXT(ROUND(D100,2),"0.00")&amp;", "&amp;TEXT(ROUND(D101,2),"0.00")&amp;", "&amp;TEXT(ROUND(D102,2),"0.00")&amp;", "&amp;TEXT(ROUND(D103,2),"0.00")&amp;", "&amp;TEXT(ROUND(D104,2),"0.00")&amp;", "&amp;TEXT(ROUND(D105,2),"0.00")&amp;", "&amp;TEXT(ROUND(D106,2),"0.00")&amp;", "&amp;TEXT(ROUND(D107,2),"0.00")&amp;", "&amp;TEXT(ROUND(D108,2),"0.00")&amp;", "&amp;TEXT(ROUND(D109,2),"0.00")&amp;"}"</f>
+        <v>{0.00, 1.00, 2.00, 3.00, 4.00, 4.17, 4.33, 4.50, 4.67, 4.83, 5.00}</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>7</v>
+      </c>
+      <c r="B115" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E115" s="41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C116" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C84" s="2">
+      <c r="D116" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E116" s="47">
+        <v>0.1333</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C117" s="2">
         <v>0</v>
       </c>
-      <c r="D84" s="49">
+      <c r="D117" s="49">
         <f>$B$2</f>
         <v>0</v>
       </c>
-      <c r="E84" s="48">
-        <f>(D91-D86)/5</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C85" s="2">
-        <f>C84+10</f>
+      <c r="E117" s="43">
+        <f>C120</f>
+        <v>30</v>
+      </c>
+      <c r="F117" s="45">
+        <f>D120</f>
+        <v>3.9990000000000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C118" s="2">
+        <f>C117+10</f>
         <v>10</v>
       </c>
-      <c r="D85" s="49">
-        <f>D84</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C86" s="2">
-        <f t="shared" ref="C86:C94" si="10">C85+10</f>
+      <c r="D118" s="49">
+        <f>C118*$E$116+$D$117</f>
+        <v>1.333</v>
+      </c>
+      <c r="E118" s="43">
+        <f>C127</f>
+        <v>100</v>
+      </c>
+      <c r="F118" s="43">
+        <f>D127</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C119" s="2">
+        <f t="shared" ref="C119:C127" si="9">C118+10</f>
         <v>20</v>
       </c>
-      <c r="D86" s="49">
-        <f>D85</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C87" s="2">
+      <c r="D119" s="49">
+        <f t="shared" ref="D119:D120" si="10">C119*$E$116+$D$117</f>
+        <v>2.6659999999999999</v>
+      </c>
+      <c r="E119" s="46">
+        <f>SLOPE(F117:F118,E117:E118)</f>
+        <v>1.4299999999999998E-2</v>
+      </c>
+      <c r="F119" s="43">
+        <f>INTERCEPT(F117:F118,E117:E118)</f>
+        <v>3.5700000000000003</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C120" s="2">
+        <f t="shared" si="9"/>
+        <v>30</v>
+      </c>
+      <c r="D120" s="49">
         <f t="shared" si="10"/>
-        <v>30</v>
-      </c>
-      <c r="D87" s="49">
-        <f>D86+$E$84</f>
-        <v>1</v>
-      </c>
-      <c r="P87" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C88" s="2">
-        <f t="shared" si="10"/>
+        <v>3.9990000000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C121" s="2">
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
-      <c r="D88" s="49">
-        <f t="shared" ref="D88:D90" si="11">D87+$E$84</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C89" s="2">
-        <f t="shared" si="10"/>
+      <c r="D121" s="49">
+        <f>C121*$E$119+$F$119</f>
+        <v>4.1420000000000003</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C122" s="2">
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
-      <c r="D89" s="49">
+      <c r="D122" s="49">
+        <f t="shared" ref="D122:D126" si="11">C122*$E$119+$F$119</f>
+        <v>4.2850000000000001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C123" s="2">
+        <f t="shared" si="9"/>
+        <v>60</v>
+      </c>
+      <c r="D123" s="49">
         <f t="shared" si="11"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C90" s="2">
-        <f t="shared" si="10"/>
-        <v>60</v>
-      </c>
-      <c r="D90" s="49">
+        <v>4.4279999999999999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C124" s="2">
+        <f t="shared" si="9"/>
+        <v>70</v>
+      </c>
+      <c r="D124" s="49">
         <f t="shared" si="11"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C91" s="2">
-        <f t="shared" si="10"/>
-        <v>70</v>
-      </c>
-      <c r="D91" s="49">
-        <f>D94</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C92" s="2">
-        <f t="shared" si="10"/>
+        <v>4.5709999999999997</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C125" s="2">
+        <f t="shared" si="9"/>
         <v>80</v>
       </c>
-      <c r="D92" s="49">
-        <f>D94</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C93" s="2">
-        <f t="shared" si="10"/>
+      <c r="D125" s="49">
+        <f t="shared" si="11"/>
+        <v>4.7140000000000004</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C126" s="2">
+        <f t="shared" si="9"/>
         <v>90</v>
       </c>
-      <c r="D93" s="49">
-        <f>D94</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C94" s="2">
-        <f t="shared" si="10"/>
+      <c r="D126" s="49">
+        <f t="shared" si="11"/>
+        <v>4.8570000000000002</v>
+      </c>
+      <c r="F126" s="50"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C127" s="2">
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
-      <c r="D94" s="49">
+      <c r="D127" s="49">
         <f>$C$2</f>
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="D95" s="44"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C97" s="40" t="s">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C130" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D130" s="51" t="str">
+        <f>"{"&amp;TEXT(ROUND(D117,2),"0.00")&amp;", "&amp;TEXT(ROUND(D118,2),"0.00")&amp;", "&amp;TEXT(ROUND(D119,2),"0.00")&amp;", "&amp;TEXT(ROUND(D120,2),"0.00")&amp;", "&amp;TEXT(ROUND(D121,2),"0.00")&amp;", "&amp;TEXT(ROUND(D122,2),"0.00")&amp;", "&amp;TEXT(ROUND(D123,2),"0.00")&amp;", "&amp;TEXT(ROUND(D124,2),"0.00")&amp;", "&amp;TEXT(ROUND(D125,2),"0.00")&amp;", "&amp;TEXT(ROUND(D126,2),"0.00")&amp;", "&amp;TEXT(ROUND(D127,2),"0.00")&amp;"}"</f>
+        <v>{0.00, 1.33, 2.67, 4.00, 4.14, 4.29, 4.43, 4.57, 4.71, 4.86, 5.00}</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>8</v>
+      </c>
+      <c r="B135" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="C135" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D97" s="51" t="str">
-        <f>"{"&amp;TEXT(ROUND(D84,2),"0.00")&amp;", "&amp;TEXT(ROUND(D85,2),"0.00")&amp;", "&amp;TEXT(ROUND(D86,2),"0.00")&amp;", "&amp;TEXT(ROUND(D87,2),"0.00")&amp;", "&amp;TEXT(ROUND(D88,2),"0.00")&amp;", "&amp;TEXT(ROUND(D89,2),"0.00")&amp;", "&amp;TEXT(ROUND(D90,2),"0.00")&amp;", "&amp;TEXT(ROUND(D91,2),"0.00")&amp;", "&amp;TEXT(ROUND(D92,2),"0.00")&amp;", "&amp;TEXT(ROUND(D93,2),"0.00")&amp;", "&amp;TEXT(ROUND(D94,2),"0.00")&amp;"}"</f>
-        <v>{0.00, 0.00, 0.00, 1.00, 2.00, 3.00, 4.00, 5.00, 5.00, 5.00, 5.00}</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <v>6</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C101" s="2" t="s">
+      <c r="E135" s="41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C136" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D101" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C102" s="2">
+      <c r="D136" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E136" s="47">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C137" s="2">
         <v>0</v>
       </c>
-      <c r="D102" s="49">
+      <c r="D137" s="49">
         <f>$B$2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C103" s="2">
-        <f>C102+10</f>
+      <c r="E137" s="43">
+        <f>C139</f>
+        <v>20</v>
+      </c>
+      <c r="F137" s="43">
+        <f>D139</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C138" s="2">
+        <f>C137+10</f>
         <v>10</v>
       </c>
-      <c r="D103" s="49">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C104" s="2">
-        <f t="shared" ref="C104:C112" si="12">C103+10</f>
+      <c r="D138" s="49">
+        <f>C138*$E$136 +$D$137</f>
+        <v>2</v>
+      </c>
+      <c r="E138" s="43">
+        <f>C147</f>
+        <v>100</v>
+      </c>
+      <c r="F138" s="43">
+        <f>D147</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C139" s="2">
+        <f t="shared" ref="C139:C147" si="12">C138+10</f>
         <v>20</v>
       </c>
-      <c r="D104" s="49">
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C105" s="2">
+      <c r="D139" s="49">
+        <f>C139*$E$136 +$D$137</f>
+        <v>4</v>
+      </c>
+      <c r="E139" s="46">
+        <f>SLOPE(F137:F138,E137:E138)</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="F139" s="43">
+        <f>INTERCEPT(F137:F138,E137:E138)</f>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C140" s="2">
         <f t="shared" si="12"/>
         <v>30</v>
       </c>
-      <c r="D105" s="49">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C106" s="2">
+      <c r="D140" s="49">
+        <f>C140*$E$139+$F$139</f>
+        <v>4.125</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C141" s="2">
         <f t="shared" si="12"/>
         <v>40</v>
       </c>
-      <c r="D106" s="49">
-        <v>1420</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C107" s="2">
+      <c r="D141" s="49">
+        <f t="shared" ref="D141:D146" si="13">C141*$E$139+$F$139</f>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C142" s="2">
         <f t="shared" si="12"/>
         <v>50</v>
       </c>
-      <c r="D107" s="49">
-        <v>1480</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C108" s="2">
+      <c r="D142" s="49">
+        <f t="shared" si="13"/>
+        <v>4.375</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C143" s="2">
         <f t="shared" si="12"/>
         <v>60</v>
       </c>
-      <c r="D108" s="49">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C109" s="2">
+      <c r="D143" s="49">
+        <f t="shared" si="13"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C144" s="2">
         <f t="shared" si="12"/>
         <v>70</v>
       </c>
-      <c r="D109" s="49">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C110" s="2">
+      <c r="D144" s="49">
+        <f t="shared" si="13"/>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C145" s="2">
         <f t="shared" si="12"/>
         <v>80</v>
       </c>
-      <c r="D110" s="49">
-        <v>1940</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C111" s="2">
+      <c r="D145" s="49">
+        <f t="shared" si="13"/>
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C146" s="2">
         <f t="shared" si="12"/>
         <v>90</v>
       </c>
-      <c r="D111" s="49">
-        <v>2060</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C112" s="2">
+      <c r="D146" s="49">
+        <f t="shared" si="13"/>
+        <v>4.875</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C147" s="2">
         <f t="shared" si="12"/>
         <v>100</v>
       </c>
-      <c r="D112" s="49">
+      <c r="D147" s="49">
         <f>$C$2</f>
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C115" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D115" s="51" t="str">
-        <f>"{"&amp;TEXT(ROUND(D102,2),"0.00")&amp;", "&amp;TEXT(ROUND(D103,2),"0.00")&amp;", "&amp;TEXT(ROUND(D104,2),"0.00")&amp;", "&amp;TEXT(ROUND(D105,2),"0.00")&amp;", "&amp;TEXT(ROUND(D106,2),"0.00")&amp;", "&amp;TEXT(ROUND(D107,2),"0.00")&amp;", "&amp;TEXT(ROUND(D108,2),"0.00")&amp;", "&amp;TEXT(ROUND(D109,2),"0.00")&amp;", "&amp;TEXT(ROUND(D110,2),"0.00")&amp;", "&amp;TEXT(ROUND(D111,2),"0.00")&amp;", "&amp;TEXT(ROUND(D112,2),"0.00")&amp;"}"</f>
-        <v>{0.00, 1200.00, 1350.00, 1400.00, 1420.00, 1480.00, 1600.00, 1750.00, 1940.00, 2060.00, 5.00}</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119">
-        <v>7</v>
-      </c>
-      <c r="B119" s="1" t="s">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C150" s="40" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C120" s="2" t="s">
+      <c r="D150" s="51" t="str">
+        <f>"{"&amp;TEXT(ROUND(D137,2),"0.00")&amp;", "&amp;TEXT(ROUND(D138,2),"0.00")&amp;", "&amp;TEXT(ROUND(D139,2),"0.00")&amp;", "&amp;TEXT(ROUND(D140,2),"0.00")&amp;", "&amp;TEXT(ROUND(D141,2),"0.00")&amp;", "&amp;TEXT(ROUND(D142,2),"0.00")&amp;", "&amp;TEXT(ROUND(D143,2),"0.00")&amp;", "&amp;TEXT(ROUND(D144,2),"0.00")&amp;", "&amp;TEXT(ROUND(D145,2),"0.00")&amp;", "&amp;TEXT(ROUND(D146,2),"0.00")&amp;", "&amp;TEXT(ROUND(D147,2),"0.00")&amp;"}"</f>
+        <v>{0.00, 2.00, 4.00, 4.13, 4.25, 4.38, 4.50, 4.63, 4.75, 4.88, 5.00}</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>9</v>
+      </c>
+      <c r="B153" s="68" t="s">
+        <v>93</v>
+      </c>
+      <c r="C153" s="71" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C154" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D120" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C121" s="2">
+      <c r="D154" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C155" s="2">
         <v>0</v>
       </c>
-      <c r="D121" s="49">
+      <c r="D155" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C156" s="2">
+        <f>C155+10</f>
+        <v>10</v>
+      </c>
+      <c r="D156" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="E156" s="59"/>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C157" s="2">
+        <f t="shared" ref="C157:C165" si="14">C156+10</f>
+        <v>20</v>
+      </c>
+      <c r="D157" s="49">
+        <v>0.4</v>
+      </c>
+      <c r="E157" s="59"/>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C158" s="2">
+        <f t="shared" si="14"/>
+        <v>30</v>
+      </c>
+      <c r="D158" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="E158" s="59"/>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C159" s="2">
+        <f t="shared" si="14"/>
+        <v>40</v>
+      </c>
+      <c r="D159" s="49">
+        <v>0.75</v>
+      </c>
+      <c r="E159" s="59"/>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C160" s="2">
+        <f t="shared" si="14"/>
+        <v>50</v>
+      </c>
+      <c r="D160" s="49">
+        <v>1.4</v>
+      </c>
+      <c r="E160" s="59"/>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C161" s="2">
+        <f t="shared" si="14"/>
+        <v>60</v>
+      </c>
+      <c r="D161" s="49">
+        <v>2.5</v>
+      </c>
+      <c r="E161" s="59"/>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C162" s="2">
+        <f t="shared" si="14"/>
+        <v>70</v>
+      </c>
+      <c r="D162" s="49">
+        <v>3.9</v>
+      </c>
+      <c r="E162" s="59"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C163" s="2">
+        <f t="shared" si="14"/>
+        <v>80</v>
+      </c>
+      <c r="D163" s="49">
+        <v>4.7</v>
+      </c>
+      <c r="E163" s="59"/>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C164" s="2">
+        <f t="shared" si="14"/>
+        <v>90</v>
+      </c>
+      <c r="D164" s="49">
+        <v>4.95</v>
+      </c>
+      <c r="E164" s="59"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C165" s="2">
+        <f t="shared" si="14"/>
+        <v>100</v>
+      </c>
+      <c r="D165" s="49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C168" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D168" s="51" t="str">
+        <f>"{"&amp;TEXT(ROUND(D155,2),"0.00")&amp;", "&amp;TEXT(ROUND(D156,2),"0.00")&amp;", "&amp;TEXT(ROUND(D157,2),"0.00")&amp;", "&amp;TEXT(ROUND(D158,2),"0.00")&amp;", "&amp;TEXT(ROUND(D159,2),"0.00")&amp;", "&amp;TEXT(ROUND(D160,2),"0.00")&amp;", "&amp;TEXT(ROUND(D161,2),"0.00")&amp;", "&amp;TEXT(ROUND(D162,2),"0.00")&amp;", "&amp;TEXT(ROUND(D163,2),"0.00")&amp;", "&amp;TEXT(ROUND(D164,2),"0.00")&amp;", "&amp;TEXT(ROUND(D165,2),"0.00")&amp;"}"</f>
+        <v>{0.00, 0.25, 0.40, 0.50, 0.75, 1.40, 2.50, 3.90, 4.70, 4.95, 5.00}</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>10</v>
+      </c>
+      <c r="B171" s="69" t="s">
+        <v>94</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C172" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C173" s="2">
+        <v>0</v>
+      </c>
+      <c r="D173" s="49">
         <f>$B$2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C122" s="2">
-        <f>C121+10</f>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C174" s="2">
+        <f>C173+10</f>
         <v>10</v>
       </c>
-      <c r="D122" s="49">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C123" s="2">
-        <f t="shared" ref="C123:C131" si="13">C122+10</f>
+      <c r="D174" s="49">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C175" s="2">
+        <f t="shared" ref="C175:C183" si="15">C174+10</f>
         <v>20</v>
       </c>
-      <c r="D123" s="49">
-        <v>1450</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C124" s="2">
-        <f t="shared" si="13"/>
+      <c r="D175" s="49">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C176" s="2">
+        <f t="shared" si="15"/>
         <v>30</v>
       </c>
-      <c r="D124" s="49">
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C125" s="2">
-        <f t="shared" si="13"/>
+      <c r="D176" s="49">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C177" s="2">
+        <f t="shared" si="15"/>
         <v>40</v>
       </c>
-      <c r="D125" s="49">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C126" s="2">
-        <f t="shared" si="13"/>
+      <c r="D177" s="49">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C178" s="2">
+        <f t="shared" si="15"/>
         <v>50</v>
       </c>
-      <c r="D126" s="49">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C127" s="2">
-        <f t="shared" si="13"/>
+      <c r="D178" s="49">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C179" s="2">
+        <f t="shared" si="15"/>
         <v>60</v>
       </c>
-      <c r="D127" s="49">
-        <v>1620</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C128" s="2">
-        <f t="shared" si="13"/>
+      <c r="D179" s="49">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C180" s="2">
+        <f t="shared" si="15"/>
         <v>70</v>
       </c>
-      <c r="D128" s="49">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C129" s="2">
-        <f t="shared" si="13"/>
+      <c r="D180" s="49">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C181" s="2">
+        <f t="shared" si="15"/>
         <v>80</v>
       </c>
-      <c r="D129" s="49">
-        <v>1940</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C130" s="2">
-        <f t="shared" si="13"/>
+      <c r="D181" s="49">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C182" s="2">
+        <f t="shared" si="15"/>
         <v>90</v>
       </c>
-      <c r="D130" s="49">
-        <v>2060</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C131" s="2">
-        <f t="shared" si="13"/>
+      <c r="D182" s="49">
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C183" s="2">
+        <f t="shared" si="15"/>
         <v>100</v>
       </c>
-      <c r="D131" s="49">
+      <c r="D183" s="49">
         <f>$C$2</f>
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C134" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D134" s="51" t="str">
-        <f>"{"&amp;TEXT(ROUND(D121,2),"0.00")&amp;", "&amp;TEXT(ROUND(D122,2),"0.00")&amp;", "&amp;TEXT(ROUND(D123,2),"0.00")&amp;", "&amp;TEXT(ROUND(D124,2),"0.00")&amp;", "&amp;TEXT(ROUND(D125,2),"0.00")&amp;", "&amp;TEXT(ROUND(D126,2),"0.00")&amp;", "&amp;TEXT(ROUND(D127,2),"0.00")&amp;", "&amp;TEXT(ROUND(D128,2),"0.00")&amp;", "&amp;TEXT(ROUND(D129,2),"0.00")&amp;", "&amp;TEXT(ROUND(D130,2),"0.00")&amp;", "&amp;TEXT(ROUND(D131,2),"0.00")&amp;"}"</f>
-        <v>{0.00, 1250.00, 1450.00, 1550.00, 1600.00, 1600.00, 1620.00, 1750.00, 1940.00, 2060.00, 5.00}</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A137">
-        <v>8</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C138" s="2" t="s">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C186" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D186" s="51" t="str">
+        <f>"{"&amp;TEXT(ROUND(D173,2),"0.00")&amp;", "&amp;TEXT(ROUND(D174,2),"0.00")&amp;", "&amp;TEXT(ROUND(D175,2),"0.00")&amp;", "&amp;TEXT(ROUND(D176,2),"0.00")&amp;", "&amp;TEXT(ROUND(D177,2),"0.00")&amp;", "&amp;TEXT(ROUND(D178,2),"0.00")&amp;", "&amp;TEXT(ROUND(D179,2),"0.00")&amp;", "&amp;TEXT(ROUND(D180,2),"0.00")&amp;", "&amp;TEXT(ROUND(D181,2),"0.00")&amp;", "&amp;TEXT(ROUND(D182,2),"0.00")&amp;", "&amp;TEXT(ROUND(D183,2),"0.00")&amp;"}"</f>
+        <v>{0.00, 0.25, 0.40, 0.70, 1.30, 2.50, 3.80, 4.55, 4.80, 4.95, 5.00}</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <v>11</v>
+      </c>
+      <c r="B189" s="70" t="s">
+        <v>95</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C190" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D138" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C139" s="2">
+      <c r="D190" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C191" s="2">
         <v>0</v>
       </c>
-      <c r="D139" s="49">
+      <c r="D191" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C192" s="2">
+        <f>C191+10</f>
+        <v>10</v>
+      </c>
+      <c r="D192" s="49">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C193" s="2">
+        <f t="shared" ref="C193:C201" si="16">C192+10</f>
+        <v>20</v>
+      </c>
+      <c r="D193" s="49">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C194" s="2">
+        <f t="shared" si="16"/>
+        <v>30</v>
+      </c>
+      <c r="D194" s="49">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C195" s="2">
+        <f t="shared" si="16"/>
+        <v>40</v>
+      </c>
+      <c r="D195" s="49">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C196" s="2">
+        <f t="shared" si="16"/>
+        <v>50</v>
+      </c>
+      <c r="D196" s="49">
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C197" s="2">
+        <f t="shared" si="16"/>
+        <v>60</v>
+      </c>
+      <c r="D197" s="49">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C198" s="2">
+        <f t="shared" si="16"/>
+        <v>70</v>
+      </c>
+      <c r="D198" s="49">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C199" s="2">
+        <f t="shared" si="16"/>
+        <v>80</v>
+      </c>
+      <c r="D199" s="49">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C200" s="2">
+        <f t="shared" si="16"/>
+        <v>90</v>
+      </c>
+      <c r="D200" s="49">
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C201" s="2">
+        <f t="shared" si="16"/>
+        <v>100</v>
+      </c>
+      <c r="D201" s="49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C204" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D204" s="51" t="str">
+        <f>"{"&amp;TEXT(ROUND(D191,2),"0.00")&amp;", "&amp;TEXT(ROUND(D192,2),"0.00")&amp;", "&amp;TEXT(ROUND(D193,2),"0.00")&amp;", "&amp;TEXT(ROUND(D194,2),"0.00")&amp;", "&amp;TEXT(ROUND(D195,2),"0.00")&amp;", "&amp;TEXT(ROUND(D196,2),"0.00")&amp;", "&amp;TEXT(ROUND(D197,2),"0.00")&amp;", "&amp;TEXT(ROUND(D198,2),"0.00")&amp;", "&amp;TEXT(ROUND(D199,2),"0.00")&amp;", "&amp;TEXT(ROUND(D200,2),"0.00")&amp;", "&amp;TEXT(ROUND(D201,2),"0.00")&amp;"}"</f>
+        <v>{0.00, 0.20, 0.60, 1.40, 2.50, 3.65, 4.35, 4.70, 4.90, 4.95, 5.00}</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A207">
+        <v>12</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C208" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D208" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="209" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C209" s="2">
+        <v>0</v>
+      </c>
+      <c r="D209" s="49">
         <f>$B$2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C140" s="2">
-        <f>C139+10</f>
+    <row r="210" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C210" s="2">
+        <f>C209+10</f>
         <v>10</v>
       </c>
-      <c r="D140" s="49">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C141" s="2">
-        <f t="shared" ref="C141:C149" si="14">C140+10</f>
+      <c r="D210" s="49">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="211" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C211" s="2">
+        <f t="shared" ref="C211:C219" si="17">C210+10</f>
         <v>20</v>
       </c>
-      <c r="D141" s="49">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C142" s="2">
-        <f t="shared" si="14"/>
+      <c r="D211" s="49">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="212" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C212" s="2">
+        <f t="shared" si="17"/>
         <v>30</v>
       </c>
-      <c r="D142" s="49">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C143" s="2">
-        <f t="shared" si="14"/>
+      <c r="D212" s="49">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="213" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C213" s="2">
+        <f t="shared" si="17"/>
         <v>40</v>
       </c>
-      <c r="D143" s="49">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C144" s="2">
-        <f t="shared" si="14"/>
+      <c r="D213" s="49">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="214" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C214" s="2">
+        <f t="shared" si="17"/>
         <v>50</v>
       </c>
-      <c r="D144" s="49">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C145" s="2">
-        <f t="shared" si="14"/>
+      <c r="D214" s="49">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="215" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C215" s="2">
+        <f t="shared" si="17"/>
         <v>60</v>
       </c>
-      <c r="D145" s="49">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C146" s="2">
-        <f t="shared" si="14"/>
+      <c r="D215" s="49">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="216" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C216" s="2">
+        <f t="shared" si="17"/>
         <v>70</v>
       </c>
-      <c r="D146" s="49">
+      <c r="D216" s="49">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="217" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C217" s="2">
+        <f t="shared" si="17"/>
+        <v>80</v>
+      </c>
+      <c r="D217" s="49">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="218" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C218" s="2">
+        <f t="shared" si="17"/>
+        <v>90</v>
+      </c>
+      <c r="D218" s="49">
         <v>1900</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C147" s="2">
-        <f t="shared" si="14"/>
-        <v>80</v>
-      </c>
-      <c r="D147" s="49">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C148" s="2">
-        <f t="shared" si="14"/>
-        <v>90</v>
-      </c>
-      <c r="D148" s="49">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C149" s="2">
-        <f t="shared" si="14"/>
+    <row r="219" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C219" s="2">
+        <f t="shared" si="17"/>
         <v>100</v>
       </c>
-      <c r="D149" s="49">
+      <c r="D219" s="49">
         <f>$C$2</f>
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C152" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D152" s="51" t="str">
-        <f>"{"&amp;TEXT(ROUND(D139,2),"0.00")&amp;", "&amp;TEXT(ROUND(D140,2),"0.00")&amp;", "&amp;TEXT(ROUND(D141,2),"0.00")&amp;", "&amp;TEXT(ROUND(D142,2),"0.00")&amp;", "&amp;TEXT(ROUND(D143,2),"0.00")&amp;", "&amp;TEXT(ROUND(D144,2),"0.00")&amp;", "&amp;TEXT(ROUND(D145,2),"0.00")&amp;", "&amp;TEXT(ROUND(D146,2),"0.00")&amp;", "&amp;TEXT(ROUND(D147,2),"0.00")&amp;", "&amp;TEXT(ROUND(D148,2),"0.00")&amp;", "&amp;TEXT(ROUND(D149,2),"0.00")&amp;"}"</f>
-        <v>{0.00, 910.00, 930.00, 1020.00, 1200.00, 1570.00, 1790.00, 1900.00, 2000.00, 2070.00, 5.00}</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A155">
-        <v>9</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C156" s="2" t="s">
+    <row r="222" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C222" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D222" s="51" t="str">
+        <f>"{"&amp;TEXT(ROUND(D209,2),"0.00")&amp;", "&amp;TEXT(ROUND(D210,2),"0.00")&amp;", "&amp;TEXT(ROUND(D211,2),"0.00")&amp;", "&amp;TEXT(ROUND(D212,2),"0.00")&amp;", "&amp;TEXT(ROUND(D213,2),"0.00")&amp;", "&amp;TEXT(ROUND(D214,2),"0.00")&amp;", "&amp;TEXT(ROUND(D215,2),"0.00")&amp;", "&amp;TEXT(ROUND(D216,2),"0.00")&amp;", "&amp;TEXT(ROUND(D217,2),"0.00")&amp;", "&amp;TEXT(ROUND(D218,2),"0.00")&amp;", "&amp;TEXT(ROUND(D219,2),"0.00")&amp;"}"</f>
+        <v>{0.00, 1020.00, 1140.00, 1260.00, 1380.00, 1380.00, 1380.00, 1380.00, 1650.00, 1900.00, 5.00}</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A227">
+        <v>13</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E227" s="41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C228" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D156" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C157" s="2">
+      <c r="D228" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E228" s="47">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C229" s="2">
         <v>0</v>
       </c>
-      <c r="D157" s="49">
+      <c r="D229" s="49">
         <f>$B$2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C158" s="2">
-        <f>C157+10</f>
+      <c r="E229" s="43">
+        <f>C234</f>
+        <v>50</v>
+      </c>
+      <c r="F229" s="45">
+        <f>D234</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C230" s="2">
+        <f>C229+10</f>
         <v>10</v>
       </c>
-      <c r="D158" s="49">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C159" s="2">
-        <f t="shared" ref="C159:C167" si="15">C158+10</f>
+      <c r="D230" s="49">
+        <f>C230*$E$231+$F$231</f>
+        <v>0.6</v>
+      </c>
+      <c r="E230" s="43">
+        <f>C229</f>
+        <v>0</v>
+      </c>
+      <c r="F230" s="45">
+        <f>D229</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C231" s="2">
+        <f t="shared" ref="C231:C239" si="18">C230+10</f>
         <v>20</v>
       </c>
-      <c r="D159" s="49">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C160" s="2">
-        <f t="shared" si="15"/>
+      <c r="D231" s="49">
+        <f t="shared" ref="D231:D233" si="19">C231*$E$231+$F$231</f>
+        <v>1.2</v>
+      </c>
+      <c r="E231" s="46">
+        <f>SLOPE(F229:F230,E229:E230)</f>
+        <v>0.06</v>
+      </c>
+      <c r="F231" s="43">
+        <f>INTERCEPT(F229:F230,E229:E230)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C232" s="2">
+        <f t="shared" si="18"/>
         <v>30</v>
       </c>
-      <c r="D160" s="49">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C161" s="2">
-        <f t="shared" si="15"/>
+      <c r="D232" s="49">
+        <f t="shared" si="19"/>
+        <v>1.7999999999999998</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C233" s="2">
+        <f t="shared" si="18"/>
         <v>40</v>
       </c>
-      <c r="D161" s="49">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C162" s="2">
-        <f t="shared" si="15"/>
+      <c r="D233" s="49">
+        <f t="shared" si="19"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C234" s="2">
+        <f t="shared" si="18"/>
         <v>50</v>
       </c>
-      <c r="D162" s="49">
-        <v>1640</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C163" s="2">
-        <f t="shared" si="15"/>
+      <c r="D234" s="49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C235" s="2">
+        <f t="shared" si="18"/>
         <v>60</v>
       </c>
-      <c r="D163" s="49">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C164" s="2">
-        <f t="shared" si="15"/>
+      <c r="D235" s="49">
+        <f>$C235*$E$228 +$D$234</f>
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C236" s="2">
+        <f t="shared" si="18"/>
         <v>70</v>
       </c>
-      <c r="D164" s="49">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C165" s="2">
-        <f t="shared" si="15"/>
+      <c r="D236" s="49">
+        <f t="shared" ref="D236:D238" si="20">$C236*$E$228 +$D$234</f>
+        <v>3.07</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C237" s="2">
+        <f t="shared" si="18"/>
         <v>80</v>
       </c>
-      <c r="D165" s="49">
-        <v>2080</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C166" s="2">
-        <f t="shared" si="15"/>
+      <c r="D237" s="49">
+        <f t="shared" si="20"/>
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C238" s="2">
+        <f t="shared" si="18"/>
         <v>90</v>
       </c>
-      <c r="D166" s="49">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C167" s="2">
-        <f t="shared" si="15"/>
+      <c r="D238" s="49">
+        <f t="shared" si="20"/>
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C239" s="2">
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
-      <c r="D167" s="49">
+      <c r="D239" s="49">
         <f>$C$2</f>
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C170" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D170" s="51" t="str">
-        <f>"{"&amp;TEXT(ROUND(D157,2),"0.00")&amp;", "&amp;TEXT(ROUND(D158,2),"0.00")&amp;", "&amp;TEXT(ROUND(D159,2),"0.00")&amp;", "&amp;TEXT(ROUND(D160,2),"0.00")&amp;", "&amp;TEXT(ROUND(D161,2),"0.00")&amp;", "&amp;TEXT(ROUND(D162,2),"0.00")&amp;", "&amp;TEXT(ROUND(D163,2),"0.00")&amp;", "&amp;TEXT(ROUND(D164,2),"0.00")&amp;", "&amp;TEXT(ROUND(D165,2),"0.00")&amp;", "&amp;TEXT(ROUND(D166,2),"0.00")&amp;", "&amp;TEXT(ROUND(D167,2),"0.00")&amp;"}"</f>
-        <v>{0.00, 900.00, 920.00, 980.00, 1200.00, 1640.00, 1900.00, 2010.00, 2080.00, 2100.00, 5.00}</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A173">
-        <v>10</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C174" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D174" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C175" s="2">
-        <v>0</v>
-      </c>
-      <c r="D175" s="49">
-        <f>$B$2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C176" s="2">
-        <f>C175+10</f>
-        <v>10</v>
-      </c>
-      <c r="D176" s="49">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C177" s="2">
-        <f t="shared" ref="C177:C185" si="16">C176+10</f>
-        <v>20</v>
-      </c>
-      <c r="D177" s="49">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C178" s="2">
-        <f t="shared" si="16"/>
-        <v>30</v>
-      </c>
-      <c r="D178" s="49">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C179" s="2">
-        <f t="shared" si="16"/>
-        <v>40</v>
-      </c>
-      <c r="D179" s="49">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C180" s="2">
-        <f t="shared" si="16"/>
-        <v>50</v>
-      </c>
-      <c r="D180" s="49">
-        <v>1110</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C181" s="2">
-        <f t="shared" si="16"/>
+    <row r="242" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C242" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="D181" s="49">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C182" s="2">
-        <f t="shared" si="16"/>
-        <v>70</v>
-      </c>
-      <c r="D182" s="49">
-        <v>1590</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C183" s="2">
-        <f t="shared" si="16"/>
-        <v>80</v>
-      </c>
-      <c r="D183" s="49">
-        <v>1890</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C184" s="2">
-        <f t="shared" si="16"/>
-        <v>90</v>
-      </c>
-      <c r="D184" s="49">
-        <v>2090</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C185" s="2">
-        <f t="shared" si="16"/>
-        <v>100</v>
-      </c>
-      <c r="D185" s="49">
-        <f>$C$2</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C188" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D188" s="51" t="str">
-        <f>"{"&amp;TEXT(ROUND(D175,2),"0.00")&amp;", "&amp;TEXT(ROUND(D176,2),"0.00")&amp;", "&amp;TEXT(ROUND(D177,2),"0.00")&amp;", "&amp;TEXT(ROUND(D178,2),"0.00")&amp;", "&amp;TEXT(ROUND(D179,2),"0.00")&amp;", "&amp;TEXT(ROUND(D180,2),"0.00")&amp;", "&amp;TEXT(ROUND(D181,2),"0.00")&amp;", "&amp;TEXT(ROUND(D182,2),"0.00")&amp;", "&amp;TEXT(ROUND(D183,2),"0.00")&amp;", "&amp;TEXT(ROUND(D184,2),"0.00")&amp;", "&amp;TEXT(ROUND(D185,2),"0.00")&amp;"}"</f>
-        <v>{0.00, 900.00, 910.00, 930.00, 990.00, 1110.00, 1310.00, 1590.00, 1890.00, 2090.00, 5.00}</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A191">
-        <v>11</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C192" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D192" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="193" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C193" s="2">
-        <v>0</v>
-      </c>
-      <c r="D193" s="49">
-        <f>$B$2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C194" s="2">
-        <f>C193+10</f>
-        <v>10</v>
-      </c>
-      <c r="D194" s="49">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="195" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C195" s="2">
-        <f t="shared" ref="C195:C203" si="17">C194+10</f>
-        <v>20</v>
-      </c>
-      <c r="D195" s="49">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="196" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C196" s="2">
-        <f t="shared" si="17"/>
-        <v>30</v>
-      </c>
-      <c r="D196" s="49">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="197" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C197" s="2">
-        <f t="shared" si="17"/>
-        <v>40</v>
-      </c>
-      <c r="D197" s="49">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="198" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C198" s="2">
-        <f t="shared" si="17"/>
-        <v>50</v>
-      </c>
-      <c r="D198" s="49">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="199" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C199" s="2">
-        <f t="shared" si="17"/>
-        <v>60</v>
-      </c>
-      <c r="D199" s="49">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="200" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C200" s="2">
-        <f t="shared" si="17"/>
-        <v>70</v>
-      </c>
-      <c r="D200" s="49">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="201" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C201" s="2">
-        <f t="shared" si="17"/>
-        <v>80</v>
-      </c>
-      <c r="D201" s="49">
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="202" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C202" s="2">
-        <f t="shared" si="17"/>
-        <v>90</v>
-      </c>
-      <c r="D202" s="49">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="203" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C203" s="2">
-        <f t="shared" si="17"/>
-        <v>100</v>
-      </c>
-      <c r="D203" s="49">
-        <f>$C$2</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="206" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C206" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D206" s="51" t="str">
-        <f>"{"&amp;TEXT(ROUND(D193,2),"0.00")&amp;", "&amp;TEXT(ROUND(D194,2),"0.00")&amp;", "&amp;TEXT(ROUND(D195,2),"0.00")&amp;", "&amp;TEXT(ROUND(D196,2),"0.00")&amp;", "&amp;TEXT(ROUND(D197,2),"0.00")&amp;", "&amp;TEXT(ROUND(D198,2),"0.00")&amp;", "&amp;TEXT(ROUND(D199,2),"0.00")&amp;", "&amp;TEXT(ROUND(D200,2),"0.00")&amp;", "&amp;TEXT(ROUND(D201,2),"0.00")&amp;", "&amp;TEXT(ROUND(D202,2),"0.00")&amp;", "&amp;TEXT(ROUND(D203,2),"0.00")&amp;"}"</f>
-        <v>{0.00, 900.00, 910.00, 920.00, 930.00, 980.00, 1100.00, 1300.00, 1550.00, 1800.00, 5.00}</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A209">
-        <v>12</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C210" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D210" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C211" s="2">
-        <v>0</v>
-      </c>
-      <c r="D211" s="49">
-        <f>$B$2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C212" s="2">
-        <f>C211+10</f>
-        <v>10</v>
-      </c>
-      <c r="D212" s="49">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C213" s="2">
-        <f t="shared" ref="C213:C221" si="18">C212+10</f>
-        <v>20</v>
-      </c>
-      <c r="D213" s="49">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C214" s="2">
-        <f t="shared" si="18"/>
-        <v>30</v>
-      </c>
-      <c r="D214" s="49">
-        <v>1260</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C215" s="2">
-        <f t="shared" si="18"/>
-        <v>40</v>
-      </c>
-      <c r="D215" s="49">
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C216" s="2">
-        <f t="shared" si="18"/>
-        <v>50</v>
-      </c>
-      <c r="D216" s="49">
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C217" s="2">
-        <f t="shared" si="18"/>
-        <v>60</v>
-      </c>
-      <c r="D217" s="49">
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C218" s="2">
-        <f t="shared" si="18"/>
-        <v>70</v>
-      </c>
-      <c r="D218" s="49">
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C219" s="2">
-        <f t="shared" si="18"/>
-        <v>80</v>
-      </c>
-      <c r="D219" s="49">
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C220" s="2">
-        <f t="shared" si="18"/>
-        <v>90</v>
-      </c>
-      <c r="D220" s="49">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C221" s="2">
-        <f t="shared" si="18"/>
-        <v>100</v>
-      </c>
-      <c r="D221" s="49">
-        <f>$C$2</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C224" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D224" s="51" t="str">
-        <f>"{"&amp;TEXT(ROUND(D211,2),"0.00")&amp;", "&amp;TEXT(ROUND(D212,2),"0.00")&amp;", "&amp;TEXT(ROUND(D213,2),"0.00")&amp;", "&amp;TEXT(ROUND(D214,2),"0.00")&amp;", "&amp;TEXT(ROUND(D215,2),"0.00")&amp;", "&amp;TEXT(ROUND(D216,2),"0.00")&amp;", "&amp;TEXT(ROUND(D217,2),"0.00")&amp;", "&amp;TEXT(ROUND(D218,2),"0.00")&amp;", "&amp;TEXT(ROUND(D219,2),"0.00")&amp;", "&amp;TEXT(ROUND(D220,2),"0.00")&amp;", "&amp;TEXT(ROUND(D221,2),"0.00")&amp;"}"</f>
-        <v>{0.00, 1020.00, 1140.00, 1260.00, 1380.00, 1380.00, 1380.00, 1380.00, 1650.00, 1900.00, 5.00}</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A229">
-        <v>13</v>
-      </c>
-      <c r="B229" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C229" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E229" s="41" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C230" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D230" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E230" s="47">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C231" s="2">
-        <v>0</v>
-      </c>
-      <c r="D231" s="49">
-        <f>$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="E231" s="43">
-        <f>C236</f>
-        <v>50</v>
-      </c>
-      <c r="F231" s="45">
-        <f>D236</f>
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C232" s="2">
-        <f>C231+10</f>
-        <v>10</v>
-      </c>
-      <c r="D232" s="49">
-        <f>C232*$E$233+$F$233</f>
-        <v>220</v>
-      </c>
-      <c r="E232" s="43">
-        <f>C231</f>
-        <v>0</v>
-      </c>
-      <c r="F232" s="45">
-        <f>D231</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C233" s="2">
-        <f t="shared" ref="C233:C241" si="19">C232+10</f>
-        <v>20</v>
-      </c>
-      <c r="D233" s="49">
-        <f t="shared" ref="D233:D235" si="20">C233*$E$233+$F$233</f>
-        <v>440</v>
-      </c>
-      <c r="E233" s="46">
-        <f>SLOPE(F231:F232,E231:E232)</f>
-        <v>22</v>
-      </c>
-      <c r="F233" s="43">
-        <f>INTERCEPT(F231:F232,E231:E232)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C234" s="2">
-        <f t="shared" si="19"/>
-        <v>30</v>
-      </c>
-      <c r="D234" s="49">
-        <f t="shared" si="20"/>
-        <v>660</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C235" s="2">
-        <f t="shared" si="19"/>
-        <v>40</v>
-      </c>
-      <c r="D235" s="49">
-        <f t="shared" si="20"/>
-        <v>880</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C236" s="2">
-        <f t="shared" si="19"/>
-        <v>50</v>
-      </c>
-      <c r="D236" s="49">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C237" s="2">
-        <f t="shared" si="19"/>
-        <v>60</v>
-      </c>
-      <c r="D237" s="49">
-        <f>$C237*$E$230 +$D$236</f>
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C238" s="2">
-        <f t="shared" si="19"/>
-        <v>70</v>
-      </c>
-      <c r="D238" s="49">
-        <f t="shared" ref="D238:D240" si="21">$C238*$E$230 +$D$236</f>
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C239" s="2">
-        <f t="shared" si="19"/>
-        <v>80</v>
-      </c>
-      <c r="D239" s="49">
-        <f t="shared" si="21"/>
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C240" s="2">
-        <f t="shared" si="19"/>
-        <v>90</v>
-      </c>
-      <c r="D240" s="49">
-        <f t="shared" si="21"/>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="241" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C241" s="2">
-        <f t="shared" si="19"/>
-        <v>100</v>
-      </c>
-      <c r="D241" s="49">
-        <f>$C$2</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="244" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C244" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D244" s="51" t="str">
-        <f>"{"&amp;TEXT(ROUND(D231,2),"0.00")&amp;", "&amp;TEXT(ROUND(D232,2),"0.00")&amp;", "&amp;TEXT(ROUND(D233,2),"0.00")&amp;", "&amp;TEXT(ROUND(D234,2),"0.00")&amp;", "&amp;TEXT(ROUND(D235,2),"0.00")&amp;", "&amp;TEXT(ROUND(D236,2),"0.00")&amp;", "&amp;TEXT(ROUND(D237,2),"0.00")&amp;", "&amp;TEXT(ROUND(D238,2),"0.00")&amp;", "&amp;TEXT(ROUND(D239,2),"0.00")&amp;", "&amp;TEXT(ROUND(D240,2),"0.00")&amp;", "&amp;TEXT(ROUND(D241,2),"0.00")&amp;"}"</f>
-        <v>{0.00, 220.00, 440.00, 660.00, 880.00, 1100.00, 1700.00, 1800.00, 1900.00, 2000.00, 5.00}</v>
+      <c r="D242" s="51" t="str">
+        <f>"{"&amp;TEXT(ROUND(D229,2),"0.00")&amp;", "&amp;TEXT(ROUND(D230,2),"0.00")&amp;", "&amp;TEXT(ROUND(D231,2),"0.00")&amp;", "&amp;TEXT(ROUND(D232,2),"0.00")&amp;", "&amp;TEXT(ROUND(D233,2),"0.00")&amp;", "&amp;TEXT(ROUND(D234,2),"0.00")&amp;", "&amp;TEXT(ROUND(D235,2),"0.00")&amp;", "&amp;TEXT(ROUND(D236,2),"0.00")&amp;", "&amp;TEXT(ROUND(D237,2),"0.00")&amp;", "&amp;TEXT(ROUND(D238,2),"0.00")&amp;", "&amp;TEXT(ROUND(D239,2),"0.00")&amp;"}"</f>
+        <v>{0.00, 0.60, 1.20, 1.80, 2.40, 3.00, 3.06, 3.07, 3.08, 3.09, 5.00}</v>
       </c>
     </row>
   </sheetData>
@@ -18981,21 +19148,21 @@
   <sheetData>
     <row r="1" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C2" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="57"/>
+      <c r="C2" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="58"/>
     </row>
     <row r="3" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.3">
@@ -19007,17 +19174,17 @@
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C5" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="57"/>
+      <c r="C5" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="58"/>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.3">
@@ -19030,21 +19197,21 @@
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C11" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="57"/>
+      <c r="C11" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="58"/>
     </row>
     <row r="12" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.3">
@@ -19056,17 +19223,17 @@
       </c>
     </row>
     <row r="14" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C14" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="57"/>
+      <c r="C14" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="58"/>
     </row>
     <row r="15" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C15" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.3">

</xml_diff>